<commit_message>
Filter and text edits
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="730">
   <si>
     <t>Last</t>
   </si>
@@ -1685,9 +1685,6 @@
     <t>Director*</t>
   </si>
   <si>
-    <t>Black</t>
-  </si>
-  <si>
     <t>Jordan Blanchard Capital</t>
   </si>
   <si>
@@ -2214,6 +2211,9 @@
   </si>
   <si>
     <t>Auckland</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2282,8 +2282,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2328,7 +2332,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2347,6 +2351,8 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2365,6 +2371,8 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2701,9 +2709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2722,16 +2728,16 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -2740,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -2752,7 +2758,7 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L1" t="s">
         <v>526</v>
@@ -2776,19 +2782,28 @@
         <v>238</v>
       </c>
       <c r="F2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H2" t="s">
+        <v>554</v>
+      </c>
+      <c r="I2" t="s">
         <v>555</v>
-      </c>
-      <c r="I2" t="s">
-        <v>556</v>
       </c>
       <c r="J2" t="s">
         <v>537</v>
+      </c>
+      <c r="K2" t="s">
+        <v>729</v>
+      </c>
+      <c r="L2" t="s">
+        <v>729</v>
+      </c>
+      <c r="M2" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
@@ -2809,16 +2824,16 @@
         <v>393</v>
       </c>
       <c r="G3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I3" t="s">
         <v>394</v>
       </c>
       <c r="J3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
@@ -2836,19 +2851,19 @@
         <v>273</v>
       </c>
       <c r="F4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I4" t="s">
         <v>454</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1">
@@ -2866,13 +2881,13 @@
         <v>247</v>
       </c>
       <c r="F5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="H5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I5" t="s">
         <v>248</v>
@@ -2899,13 +2914,13 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I6" t="s">
         <v>460</v>
@@ -2926,16 +2941,16 @@
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="J7" t="s">
         <v>527</v>
@@ -2956,13 +2971,13 @@
         <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I8" t="s">
         <v>400</v>
@@ -2983,25 +2998,25 @@
         <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G9" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J9" t="s">
         <v>550</v>
       </c>
       <c r="K9" t="s">
+        <v>562</v>
+      </c>
+      <c r="L9" t="s">
         <v>563</v>
-      </c>
-      <c r="L9" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
@@ -3022,13 +3037,13 @@
         <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I10" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="J10" t="s">
         <v>550</v>
@@ -3049,19 +3064,19 @@
         <v>500</v>
       </c>
       <c r="F11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="J11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1">
@@ -3079,16 +3094,16 @@
         <v>235</v>
       </c>
       <c r="F12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G12" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H12" t="s">
         <v>524</v>
       </c>
       <c r="I12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J12" t="s">
         <v>21</v>
@@ -3096,7 +3111,7 @@
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
@@ -3115,13 +3130,13 @@
         <v>373</v>
       </c>
       <c r="G13" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H13" t="s">
         <v>524</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>527</v>
@@ -3145,10 +3160,10 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G14" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H14" t="s">
         <v>524</v>
@@ -3157,7 +3172,7 @@
         <v>533</v>
       </c>
       <c r="J14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
@@ -3178,7 +3193,7 @@
         <v>212</v>
       </c>
       <c r="F15" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G15" t="s">
         <v>212</v>
@@ -3209,19 +3224,19 @@
         <v>115</v>
       </c>
       <c r="F16" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G16" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H16" t="s">
         <v>524</v>
       </c>
       <c r="I16" t="s">
+        <v>600</v>
+      </c>
+      <c r="J16" t="s">
         <v>601</v>
-      </c>
-      <c r="J16" t="s">
-        <v>602</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>
@@ -3248,13 +3263,13 @@
         <v>350</v>
       </c>
       <c r="G17" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>524</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>550</v>
@@ -3281,10 +3296,10 @@
         <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G18" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H18" t="s">
         <v>524</v>
@@ -3314,19 +3329,19 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G19" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H19" t="s">
         <v>524</v>
       </c>
       <c r="I19" t="s">
+        <v>659</v>
+      </c>
+      <c r="J19" t="s">
         <v>660</v>
-      </c>
-      <c r="J19" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
@@ -3347,13 +3362,13 @@
         <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H20" t="s">
         <v>524</v>
       </c>
       <c r="I20" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J20" t="s">
         <v>527</v>
@@ -3374,10 +3389,10 @@
         <v>222</v>
       </c>
       <c r="F21" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G21" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H21" t="s">
         <v>524</v>
@@ -3410,13 +3425,13 @@
         <v>356</v>
       </c>
       <c r="G22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H22" t="s">
         <v>524</v>
       </c>
       <c r="I22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1">
@@ -3437,16 +3452,16 @@
         <v>273</v>
       </c>
       <c r="F23" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G23" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H23" t="s">
         <v>524</v>
       </c>
       <c r="I23" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1">
@@ -3467,19 +3482,19 @@
         <v>470</v>
       </c>
       <c r="F24" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G24" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H24" t="s">
         <v>524</v>
       </c>
       <c r="I24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J24" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3500,19 +3515,19 @@
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G25" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H25" t="s">
         <v>524</v>
       </c>
       <c r="I25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J25" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K25"/>
       <c r="L25"/>
@@ -3533,10 +3548,10 @@
         <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G26" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H26" t="s">
         <v>524</v>
@@ -3564,19 +3579,19 @@
         <v>261</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>524</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -3600,7 +3615,7 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H28" t="s">
         <v>524</v>
@@ -3614,7 +3629,7 @@
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B29" t="s">
         <v>388</v>
@@ -3630,16 +3645,16 @@
         <v>483</v>
       </c>
       <c r="F29" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G29" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H29" t="s">
         <v>524</v>
       </c>
       <c r="I29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J29" t="s">
         <v>532</v>
@@ -3663,7 +3678,7 @@
         <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H30" t="s">
         <v>524</v>
@@ -3672,7 +3687,7 @@
         <v>543</v>
       </c>
       <c r="J30" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1">
@@ -3680,7 +3695,7 @@
         <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -3690,22 +3705,19 @@
         <v>244</v>
       </c>
       <c r="F31" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G31" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H31" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I31" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J31" t="s">
-        <v>557</v>
-      </c>
-      <c r="M31" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1">
@@ -3723,16 +3735,16 @@
         <v>273</v>
       </c>
       <c r="F32" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G32" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I32" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>550</v>
@@ -3753,24 +3765,24 @@
         <v>273</v>
       </c>
       <c r="F33" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G33" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
       <c r="A34" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B34" t="s">
         <v>430</v>
@@ -3786,16 +3798,16 @@
         <v>431</v>
       </c>
       <c r="F34" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G34" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H34" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I34" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J34" t="s">
         <v>532</v>
@@ -3803,7 +3815,7 @@
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
       <c r="A35" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B35" t="s">
         <v>382</v>
@@ -3816,16 +3828,16 @@
         <v>129</v>
       </c>
       <c r="F35" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G35" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H35" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I35" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="J35" t="s">
         <v>21</v>
@@ -3847,19 +3859,19 @@
         <v>488</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>489</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -3889,7 +3901,7 @@
         <v>531</v>
       </c>
       <c r="I37" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J37" t="s">
         <v>550</v>
@@ -3913,19 +3925,19 @@
         <v>456</v>
       </c>
       <c r="F38" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G38" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H38" t="s">
         <v>531</v>
       </c>
       <c r="I38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J38" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1">
@@ -3946,10 +3958,10 @@
         <v>50</v>
       </c>
       <c r="F39" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G39" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H39" t="s">
         <v>531</v>
@@ -3958,7 +3970,7 @@
         <v>65</v>
       </c>
       <c r="J39" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1">
@@ -3979,7 +3991,7 @@
         <v>69</v>
       </c>
       <c r="G40" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="H40" t="s">
         <v>531</v>
@@ -4006,19 +4018,19 @@
         <v>456</v>
       </c>
       <c r="F41" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G41" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H41" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I41" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J41" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4037,19 +4049,19 @@
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G42" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H42" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I42" t="s">
         <v>384</v>
       </c>
       <c r="J42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
@@ -4073,16 +4085,19 @@
         <v>77</v>
       </c>
       <c r="G43" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H43" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I43" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J43" t="s">
-        <v>687</v>
+        <v>686</v>
+      </c>
+      <c r="M43" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4101,19 +4116,19 @@
         <v>407</v>
       </c>
       <c r="F44" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G44" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H44" t="s">
+        <v>627</v>
+      </c>
+      <c r="I44" t="s">
+        <v>629</v>
+      </c>
+      <c r="J44" t="s">
         <v>628</v>
-      </c>
-      <c r="I44" t="s">
-        <v>630</v>
-      </c>
-      <c r="J44" t="s">
-        <v>629</v>
       </c>
       <c r="K44"/>
       <c r="L44"/>
@@ -4137,13 +4152,13 @@
         <v>77</v>
       </c>
       <c r="G45" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H45" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I45" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J45" t="s">
         <v>481</v>
@@ -4164,16 +4179,16 @@
         <v>232</v>
       </c>
       <c r="F46" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G46" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H46" t="s">
         <v>530</v>
       </c>
       <c r="I46" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J46" t="s">
         <v>537</v>
@@ -4194,13 +4209,13 @@
         <v>212</v>
       </c>
       <c r="F47" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G47" t="s">
         <v>212</v>
       </c>
       <c r="H47" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>301</v>
@@ -4227,13 +4242,13 @@
         <v>441</v>
       </c>
       <c r="G48" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H48" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I48" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="J48" t="s">
         <v>550</v>
@@ -4254,13 +4269,13 @@
         <v>50</v>
       </c>
       <c r="F49" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G49" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H49" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I49" t="s">
         <v>397</v>
@@ -4284,16 +4299,16 @@
         <v>257</v>
       </c>
       <c r="F50" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G50" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H50" t="s">
+        <v>559</v>
+      </c>
+      <c r="I50" t="s">
         <v>560</v>
-      </c>
-      <c r="I50" t="s">
-        <v>561</v>
       </c>
       <c r="J50" t="s">
         <v>21</v>
@@ -4314,13 +4329,13 @@
         <v>376</v>
       </c>
       <c r="F51" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G51" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H51" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I51" t="s">
         <v>377</v>
@@ -4347,13 +4362,13 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G52" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H52" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I52" t="s">
         <v>467</v>
@@ -4374,7 +4389,7 @@
         <v xml:space="preserve">Rob Light </v>
       </c>
       <c r="H53" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I53" t="s">
         <v>521</v>
@@ -4401,13 +4416,13 @@
         <v>50</v>
       </c>
       <c r="F54" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G54" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H54" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I54" t="s">
         <v>316</v>
@@ -4434,13 +4449,13 @@
         <v>50</v>
       </c>
       <c r="F55" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G55" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H55" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I55" t="s">
         <v>316</v>
@@ -4451,7 +4466,7 @@
     </row>
     <row r="56" spans="1:13" ht="15" customHeight="1">
       <c r="A56" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B56" t="s">
         <v>314</v>
@@ -4464,24 +4479,24 @@
         <v>408</v>
       </c>
       <c r="F56" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G56" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H56" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I56" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J56" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A57" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B57" t="s">
         <v>324</v>
@@ -4495,19 +4510,19 @@
         <v>50</v>
       </c>
       <c r="F57" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G57" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H57" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I57" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J57" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K57"/>
       <c r="L57"/>
@@ -4528,19 +4543,19 @@
         <v>344</v>
       </c>
       <c r="F58" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G58" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H58" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I58" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J58" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1">
@@ -4558,19 +4573,19 @@
         <v>50</v>
       </c>
       <c r="F59" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G59" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H59" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I59" t="s">
+        <v>593</v>
+      </c>
+      <c r="J59" t="s">
         <v>594</v>
-      </c>
-      <c r="J59" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1">
@@ -4588,19 +4603,19 @@
         <v>307</v>
       </c>
       <c r="F60" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G60" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H60" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I60" t="s">
         <v>305</v>
       </c>
       <c r="J60" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15" customHeight="1">
@@ -4618,19 +4633,19 @@
         <v>50</v>
       </c>
       <c r="F61" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G61" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H61" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I61" t="s">
         <v>305</v>
       </c>
       <c r="J61" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1">
@@ -4648,25 +4663,25 @@
         <v>309</v>
       </c>
       <c r="F62" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G62" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H62" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I62" t="s">
+        <v>575</v>
+      </c>
+      <c r="J62" t="s">
         <v>576</v>
-      </c>
-      <c r="J62" t="s">
-        <v>577</v>
       </c>
       <c r="K62" t="s">
         <v>310</v>
       </c>
       <c r="L62" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1">
@@ -4684,16 +4699,16 @@
         <v>309</v>
       </c>
       <c r="F63" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G63" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H63" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I63" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>532</v>
@@ -4701,10 +4716,10 @@
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1">
       <c r="A64" t="s">
+        <v>634</v>
+      </c>
+      <c r="B64" t="s">
         <v>635</v>
-      </c>
-      <c r="B64" t="s">
-        <v>636</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
@@ -4714,16 +4729,16 @@
         <v>212</v>
       </c>
       <c r="F64" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G64" t="s">
         <v>212</v>
       </c>
       <c r="H64" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I64" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J64" t="s">
         <v>21</v>
@@ -4744,13 +4759,13 @@
         <v>50</v>
       </c>
       <c r="F65" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G65" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H65" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I65" t="s">
         <v>544</v>
@@ -4761,7 +4776,7 @@
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1">
       <c r="A66" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B66" t="s">
         <v>477</v>
@@ -4774,19 +4789,19 @@
         <v>222</v>
       </c>
       <c r="F66" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G66" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H66" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I66" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J66" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="15" customHeight="1">
@@ -4807,22 +4822,22 @@
         <v>270</v>
       </c>
       <c r="F67" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G67" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H67" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I67" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="J67" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K67" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L67" t="s">
         <v>21</v>
@@ -4843,13 +4858,13 @@
         <v>232</v>
       </c>
       <c r="F68" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G68" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H68" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I68" t="s">
         <v>233</v>
@@ -4874,13 +4889,13 @@
         <v>212</v>
       </c>
       <c r="F69" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G69" t="s">
         <v>212</v>
       </c>
       <c r="H69" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I69" t="s">
         <v>546</v>
@@ -4907,16 +4922,16 @@
         <v>270</v>
       </c>
       <c r="F70" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G70" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H70" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I70" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J70" t="s">
         <v>527</v>
@@ -4937,16 +4952,16 @@
         <v>50</v>
       </c>
       <c r="F71" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G71" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H71" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I71" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="15" customHeight="1">
@@ -4964,25 +4979,25 @@
         <v>265</v>
       </c>
       <c r="F72" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G72" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H72" t="s">
+        <v>564</v>
+      </c>
+      <c r="I72" t="s">
         <v>565</v>
       </c>
-      <c r="I72" t="s">
-        <v>566</v>
-      </c>
       <c r="J72" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K72" t="s">
         <v>266</v>
       </c>
       <c r="L72" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="15" customHeight="1">
@@ -5000,19 +5015,19 @@
         <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G73" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H73" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I73" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -5035,13 +5050,13 @@
         <v>77</v>
       </c>
       <c r="G74" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H74" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I74" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="J74" t="s">
         <v>21</v>
@@ -5062,22 +5077,22 @@
         <v>207</v>
       </c>
       <c r="F75" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G75" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H75" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I75" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J75" t="s">
         <v>523</v>
       </c>
       <c r="M75" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15" customHeight="1">
@@ -5098,16 +5113,16 @@
         <v>50</v>
       </c>
       <c r="F76" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G76" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H76" t="s">
         <v>529</v>
       </c>
       <c r="I76" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J76" t="s">
         <v>532</v>
@@ -5128,16 +5143,16 @@
         <v>307</v>
       </c>
       <c r="F77" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G77" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H77" t="s">
         <v>529</v>
       </c>
       <c r="I77" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J77" t="s">
         <v>527</v>
@@ -5158,16 +5173,16 @@
         <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G78" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H78" t="s">
         <v>529</v>
       </c>
       <c r="I78" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J78" t="s">
         <v>537</v>
@@ -5188,10 +5203,10 @@
         <v>273</v>
       </c>
       <c r="F79" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G79" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H79" t="s">
         <v>529</v>
@@ -5221,10 +5236,10 @@
         <v>50</v>
       </c>
       <c r="F80" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G80" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H80" t="s">
         <v>529</v>
@@ -5251,19 +5266,19 @@
         <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G81" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H81" t="s">
         <v>529</v>
       </c>
       <c r="I81" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="J81" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="15" customHeight="1">
@@ -5281,19 +5296,19 @@
         <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G82" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H82" t="s">
         <v>529</v>
       </c>
       <c r="I82" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J82" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15" customHeight="1">
@@ -5311,10 +5326,10 @@
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G83" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H83" t="s">
         <v>529</v>
@@ -5342,19 +5357,19 @@
         <v>50</v>
       </c>
       <c r="F84" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G84" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H84" t="s">
         <v>529</v>
       </c>
       <c r="I84" t="s">
+        <v>579</v>
+      </c>
+      <c r="J84" t="s">
         <v>580</v>
-      </c>
-      <c r="J84" t="s">
-        <v>581</v>
       </c>
       <c r="K84"/>
       <c r="L84"/>
@@ -5375,10 +5390,10 @@
         <v>219</v>
       </c>
       <c r="F85" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G85" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="H85" t="s">
         <v>549</v>
@@ -5405,10 +5420,10 @@
         <v>247</v>
       </c>
       <c r="F86" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G86" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H86" t="s">
         <v>549</v>
@@ -5417,7 +5432,7 @@
         <v>387</v>
       </c>
       <c r="J86" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="15" customHeight="1">
@@ -5438,10 +5453,10 @@
         <v>436</v>
       </c>
       <c r="F87" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G87" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H87" t="s">
         <v>549</v>
@@ -5450,7 +5465,7 @@
         <v>437</v>
       </c>
       <c r="J87" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="15" customHeight="1">
@@ -5468,19 +5483,19 @@
         <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G88" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H88" t="s">
+        <v>581</v>
+      </c>
+      <c r="I88" t="s">
         <v>582</v>
       </c>
-      <c r="I88" t="s">
-        <v>583</v>
-      </c>
       <c r="J88" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="15" customHeight="1">
@@ -5498,19 +5513,19 @@
         <v>212</v>
       </c>
       <c r="F89" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G89" t="s">
         <v>212</v>
       </c>
       <c r="H89" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I89" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J89" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="15" customHeight="1">
@@ -5525,13 +5540,13 @@
         <v xml:space="preserve">Lou  Holtz </v>
       </c>
       <c r="H90" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I90" t="s">
+        <v>604</v>
+      </c>
+      <c r="J90" t="s">
         <v>605</v>
-      </c>
-      <c r="J90" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="91" spans="1:13" s="4" customFormat="1" ht="15" customHeight="1">
@@ -5550,16 +5565,16 @@
         <v>8</v>
       </c>
       <c r="F91" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G91" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H91" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I91" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="J91" t="s">
         <v>527</v>
@@ -5583,19 +5598,19 @@
         <v>50</v>
       </c>
       <c r="F92" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G92" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H92" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I92" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J92" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="15" customHeight="1">
@@ -5613,16 +5628,16 @@
         <v>8</v>
       </c>
       <c r="F93" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G93" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H93" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I93" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J93" t="s">
         <v>21</v>
@@ -5630,7 +5645,7 @@
     </row>
     <row r="94" spans="1:13" ht="15" customHeight="1">
       <c r="A94" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B94" t="s">
         <v>362</v>
@@ -5643,24 +5658,24 @@
         <v>363</v>
       </c>
       <c r="F94" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G94" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H94" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I94" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J94" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="95" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A95" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B95" t="s">
         <v>22</v>
@@ -5676,13 +5691,13 @@
         <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G95" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H95" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I95" t="s">
         <v>531</v>
@@ -5694,7 +5709,7 @@
     </row>
     <row r="96" spans="1:13" ht="15" customHeight="1">
       <c r="A96" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B96" t="s">
         <v>22</v>
@@ -5710,10 +5725,10 @@
         <v>486</v>
       </c>
       <c r="G96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H96" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I96" t="s">
         <v>531</v>
@@ -5721,7 +5736,7 @@
     </row>
     <row r="97" spans="1:13" ht="15" customHeight="1">
       <c r="A97" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B97" t="s">
         <v>22</v>
@@ -5737,13 +5752,13 @@
         <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G97" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H97" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I97" t="s">
         <v>531</v>
@@ -5767,13 +5782,13 @@
         <v>418</v>
       </c>
       <c r="F98" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G98" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H98" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I98" t="s">
         <v>518</v>
@@ -5782,7 +5797,7 @@
         <v>550</v>
       </c>
       <c r="M98" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15" customHeight="1">
@@ -5803,13 +5818,13 @@
         <v>415</v>
       </c>
       <c r="F99" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G99" t="s">
         <v>212</v>
       </c>
       <c r="H99" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I99" t="s">
         <v>416</v>
@@ -5833,13 +5848,13 @@
         <v>59</v>
       </c>
       <c r="F100" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G100" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H100" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I100" t="s">
         <v>416</v>
@@ -5850,17 +5865,17 @@
     </row>
     <row r="101" spans="1:13" ht="15" customHeight="1">
       <c r="A101" t="s">
+        <v>612</v>
+      </c>
+      <c r="B101" t="s">
         <v>613</v>
-      </c>
-      <c r="B101" t="s">
-        <v>614</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">Virginia Rometty </v>
       </c>
       <c r="H101" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I101" t="s">
         <v>416</v>
@@ -5869,7 +5884,7 @@
         <v>527</v>
       </c>
       <c r="M101" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="15" customHeight="1">
@@ -5884,16 +5899,16 @@
         <v xml:space="preserve">Jerry Yang </v>
       </c>
       <c r="E102" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F102" t="s">
         <v>77</v>
       </c>
       <c r="G102" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H102" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I102" t="s">
         <v>513</v>
@@ -5920,10 +5935,10 @@
         <v>15</v>
       </c>
       <c r="G103" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H103" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I103" t="s">
         <v>525</v>
@@ -5950,10 +5965,10 @@
         <v>15</v>
       </c>
       <c r="G104" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H104" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I104" t="s">
         <v>525</v>
@@ -5974,7 +5989,7 @@
         <v xml:space="preserve">Craig Heatley </v>
       </c>
       <c r="E105" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F105" t="s">
         <v>368</v>
@@ -5983,10 +5998,10 @@
         <v>368</v>
       </c>
       <c r="H105" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J105" s="4" t="s">
         <v>21</v>
@@ -6007,22 +6022,19 @@
         <v>8</v>
       </c>
       <c r="F106" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G106" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H106" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I106" t="s">
         <v>228</v>
       </c>
       <c r="J106" t="s">
-        <v>664</v>
-      </c>
-      <c r="M106" t="s">
-        <v>553</v>
+        <v>663</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="15" customHeight="1">
@@ -6043,16 +6055,16 @@
         <v>205</v>
       </c>
       <c r="F107" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G107" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H107" t="s">
         <v>541</v>
       </c>
       <c r="I107" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J107" t="s">
         <v>527</v>
@@ -6076,10 +6088,10 @@
         <v>71</v>
       </c>
       <c r="F108" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G108" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H108" t="s">
         <v>541</v>
@@ -6112,13 +6124,13 @@
         <v>418</v>
       </c>
       <c r="F109" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G109" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H109" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I109" t="s">
         <v>419</v>
@@ -6146,10 +6158,10 @@
         <v>497</v>
       </c>
       <c r="G110" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H110" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I110" t="s">
         <v>498</v>
@@ -6163,7 +6175,7 @@
     </row>
     <row r="111" spans="1:13" ht="15" customHeight="1">
       <c r="A111" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B111" t="s">
         <v>389</v>
@@ -6179,19 +6191,19 @@
         <v>129</v>
       </c>
       <c r="F111" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G111" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H111" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I111" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="J111" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -6277,7 +6289,7 @@
         <v>511</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>

</xml_diff>

<commit_message>
Billionaires filter, final edits
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="731">
   <si>
     <t>Last</t>
   </si>
@@ -1799,9 +1799,6 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>World's richest person</t>
-  </si>
-  <si>
     <t>Commissioner</t>
   </si>
   <si>
@@ -2217,6 +2214,9 @@
   </si>
   <si>
     <t>Philanthropy</t>
+  </si>
+  <si>
+    <t>Billionaire</t>
   </si>
 </sst>
 </file>
@@ -2728,8 +2728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2749,16 +2749,16 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -2767,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -2779,7 +2779,7 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="L1" t="s">
         <v>524</v>
@@ -2803,10 +2803,10 @@
         <v>238</v>
       </c>
       <c r="F2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H2" t="s">
         <v>552</v>
@@ -2836,10 +2836,10 @@
         <v>391</v>
       </c>
       <c r="G3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I3" t="s">
         <v>392</v>
@@ -2863,10 +2863,10 @@
         <v>273</v>
       </c>
       <c r="F4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G4" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H4" t="s">
         <v>587</v>
@@ -2893,10 +2893,10 @@
         <v>247</v>
       </c>
       <c r="F5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H5" t="s">
         <v>555</v>
@@ -2926,10 +2926,10 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H6" t="s">
         <v>555</v>
@@ -2953,16 +2953,16 @@
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G7" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H7" t="s">
         <v>555</v>
       </c>
       <c r="I7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J7" t="s">
         <v>525</v>
@@ -2983,10 +2983,10 @@
         <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H8" t="s">
         <v>555</v>
@@ -3010,10 +3010,10 @@
         <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G9" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H9" t="s">
         <v>555</v>
@@ -3049,13 +3049,13 @@
         <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I10" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J10" t="s">
         <v>548</v>
@@ -3076,19 +3076,19 @@
         <v>498</v>
       </c>
       <c r="F11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G11" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I11" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1">
@@ -3106,10 +3106,10 @@
         <v>235</v>
       </c>
       <c r="F12" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H12" t="s">
         <v>522</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
@@ -3142,7 +3142,7 @@
         <v>371</v>
       </c>
       <c r="G13" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H13" t="s">
         <v>522</v>
@@ -3172,10 +3172,10 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G14" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H14" t="s">
         <v>522</v>
@@ -3184,7 +3184,7 @@
         <v>531</v>
       </c>
       <c r="J14" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
@@ -3205,7 +3205,7 @@
         <v>212</v>
       </c>
       <c r="F15" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G15" t="s">
         <v>212</v>
@@ -3236,19 +3236,19 @@
         <v>115</v>
       </c>
       <c r="F16" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G16" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H16" t="s">
         <v>522</v>
       </c>
       <c r="I16" t="s">
+        <v>594</v>
+      </c>
+      <c r="J16" t="s">
         <v>595</v>
-      </c>
-      <c r="J16" t="s">
-        <v>596</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>
@@ -3275,13 +3275,13 @@
         <v>348</v>
       </c>
       <c r="G17" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>522</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>548</v>
@@ -3308,10 +3308,10 @@
         <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G18" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H18" t="s">
         <v>522</v>
@@ -3341,19 +3341,19 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G19" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H19" t="s">
         <v>522</v>
       </c>
       <c r="I19" t="s">
+        <v>652</v>
+      </c>
+      <c r="J19" t="s">
         <v>653</v>
-      </c>
-      <c r="J19" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
@@ -3374,13 +3374,13 @@
         <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H20" t="s">
         <v>522</v>
       </c>
       <c r="I20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J20" t="s">
         <v>525</v>
@@ -3401,10 +3401,10 @@
         <v>222</v>
       </c>
       <c r="F21" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G21" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H21" t="s">
         <v>522</v>
@@ -3437,13 +3437,13 @@
         <v>354</v>
       </c>
       <c r="G22" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H22" t="s">
         <v>522</v>
       </c>
       <c r="I22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1">
@@ -3464,16 +3464,16 @@
         <v>273</v>
       </c>
       <c r="F23" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G23" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H23" t="s">
         <v>522</v>
       </c>
       <c r="I23" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="J23" t="s">
         <v>521</v>
@@ -3497,16 +3497,16 @@
         <v>468</v>
       </c>
       <c r="F24" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G24" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H24" t="s">
         <v>522</v>
       </c>
       <c r="I24" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="J24" t="s">
         <v>561</v>
@@ -3530,10 +3530,10 @@
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H25" t="s">
         <v>522</v>
@@ -3563,10 +3563,10 @@
         <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G26" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H26" t="s">
         <v>522</v>
@@ -3594,16 +3594,16 @@
         <v>261</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>522</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>564</v>
@@ -3630,21 +3630,24 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H28" t="s">
         <v>522</v>
       </c>
       <c r="I28" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J28" t="s">
         <v>525</v>
       </c>
+      <c r="M28" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B29" t="s">
         <v>386</v>
@@ -3660,16 +3663,16 @@
         <v>481</v>
       </c>
       <c r="F29" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G29" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H29" t="s">
         <v>522</v>
       </c>
       <c r="I29" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="J29" t="s">
         <v>530</v>
@@ -3693,7 +3696,7 @@
         <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H30" t="s">
         <v>522</v>
@@ -3710,7 +3713,7 @@
         <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -3720,16 +3723,16 @@
         <v>244</v>
       </c>
       <c r="F31" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G31" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H31" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I31" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J31" t="s">
         <v>554</v>
@@ -3750,13 +3753,13 @@
         <v>273</v>
       </c>
       <c r="F32" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G32" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H32" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I32" t="s">
         <v>585</v>
@@ -3780,13 +3783,13 @@
         <v>273</v>
       </c>
       <c r="F33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H33" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I33" t="s">
         <v>585</v>
@@ -3797,7 +3800,7 @@
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
       <c r="A34" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B34" t="s">
         <v>428</v>
@@ -3813,16 +3816,16 @@
         <v>429</v>
       </c>
       <c r="F34" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G34" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H34" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I34" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J34" t="s">
         <v>530</v>
@@ -3830,7 +3833,7 @@
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
       <c r="A35" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B35" t="s">
         <v>380</v>
@@ -3843,16 +3846,16 @@
         <v>129</v>
       </c>
       <c r="F35" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G35" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I35" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J35" t="s">
         <v>21</v>
@@ -3874,13 +3877,13 @@
         <v>486</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>487</v>
@@ -3916,7 +3919,7 @@
         <v>529</v>
       </c>
       <c r="I37" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J37" t="s">
         <v>548</v>
@@ -3940,10 +3943,10 @@
         <v>454</v>
       </c>
       <c r="F38" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G38" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H38" t="s">
         <v>529</v>
@@ -3952,7 +3955,7 @@
         <v>581</v>
       </c>
       <c r="J38" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1">
@@ -3973,10 +3976,10 @@
         <v>50</v>
       </c>
       <c r="F39" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G39" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H39" t="s">
         <v>529</v>
@@ -3985,7 +3988,7 @@
         <v>65</v>
       </c>
       <c r="J39" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1">
@@ -4006,7 +4009,7 @@
         <v>69</v>
       </c>
       <c r="G40" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H40" t="s">
         <v>529</v>
@@ -4033,19 +4036,19 @@
         <v>454</v>
       </c>
       <c r="F41" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G41" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H41" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I41" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J41" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4064,19 +4067,19 @@
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G42" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I42" t="s">
         <v>382</v>
       </c>
       <c r="J42" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
@@ -4100,19 +4103,19 @@
         <v>77</v>
       </c>
       <c r="G43" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H43" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I43" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J43" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="M43" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4131,19 +4134,19 @@
         <v>405</v>
       </c>
       <c r="F44" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G44" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H44" t="s">
+        <v>621</v>
+      </c>
+      <c r="I44" t="s">
+        <v>623</v>
+      </c>
+      <c r="J44" t="s">
         <v>622</v>
-      </c>
-      <c r="I44" t="s">
-        <v>624</v>
-      </c>
-      <c r="J44" t="s">
-        <v>623</v>
       </c>
       <c r="K44"/>
       <c r="L44"/>
@@ -4167,13 +4170,13 @@
         <v>77</v>
       </c>
       <c r="G45" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H45" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I45" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J45" t="s">
         <v>479</v>
@@ -4194,10 +4197,10 @@
         <v>232</v>
       </c>
       <c r="F46" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G46" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H46" t="s">
         <v>528</v>
@@ -4224,7 +4227,7 @@
         <v>212</v>
       </c>
       <c r="F47" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G47" t="s">
         <v>212</v>
@@ -4257,13 +4260,13 @@
         <v>439</v>
       </c>
       <c r="G48" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H48" t="s">
         <v>557</v>
       </c>
       <c r="I48" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J48" t="s">
         <v>548</v>
@@ -4284,10 +4287,10 @@
         <v>50</v>
       </c>
       <c r="F49" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G49" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H49" t="s">
         <v>557</v>
@@ -4317,10 +4320,10 @@
         <v>257</v>
       </c>
       <c r="F50" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G50" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H50" t="s">
         <v>557</v>
@@ -4347,10 +4350,10 @@
         <v>374</v>
       </c>
       <c r="F51" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G51" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H51" t="s">
         <v>557</v>
@@ -4380,10 +4383,10 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G52" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H52" t="s">
         <v>557</v>
@@ -4434,10 +4437,10 @@
         <v>50</v>
       </c>
       <c r="F54" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G54" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H54" t="s">
         <v>557</v>
@@ -4467,10 +4470,10 @@
         <v>50</v>
       </c>
       <c r="F55" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G55" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H55" t="s">
         <v>557</v>
@@ -4484,7 +4487,7 @@
     </row>
     <row r="56" spans="1:13" ht="15" customHeight="1">
       <c r="A56" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B56" t="s">
         <v>313</v>
@@ -4497,16 +4500,16 @@
         <v>406</v>
       </c>
       <c r="F56" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H56" t="s">
         <v>557</v>
       </c>
       <c r="I56" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J56" t="s">
         <v>564</v>
@@ -4514,7 +4517,7 @@
     </row>
     <row r="57" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A57" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B57" t="s">
         <v>323</v>
@@ -4528,16 +4531,16 @@
         <v>50</v>
       </c>
       <c r="F57" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G57" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H57" t="s">
         <v>557</v>
       </c>
       <c r="I57" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J57" t="s">
         <v>564</v>
@@ -4561,16 +4564,16 @@
         <v>343</v>
       </c>
       <c r="F58" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G58" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H58" t="s">
         <v>557</v>
       </c>
       <c r="I58" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="J58" t="s">
         <v>575</v>
@@ -4591,10 +4594,10 @@
         <v>50</v>
       </c>
       <c r="F59" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G59" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H59" t="s">
         <v>570</v>
@@ -4621,10 +4624,10 @@
         <v>306</v>
       </c>
       <c r="F60" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G60" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H60" t="s">
         <v>570</v>
@@ -4651,10 +4654,10 @@
         <v>50</v>
       </c>
       <c r="F61" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G61" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H61" t="s">
         <v>570</v>
@@ -4681,16 +4684,16 @@
         <v>308</v>
       </c>
       <c r="F62" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G62" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H62" t="s">
         <v>570</v>
       </c>
       <c r="I62" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J62" t="s">
         <v>575</v>
@@ -4717,13 +4720,13 @@
         <v>308</v>
       </c>
       <c r="F63" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G63" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H63" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I63" t="s">
         <v>586</v>
@@ -4734,10 +4737,10 @@
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1">
       <c r="A64" t="s">
+        <v>628</v>
+      </c>
+      <c r="B64" t="s">
         <v>629</v>
-      </c>
-      <c r="B64" t="s">
-        <v>630</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
@@ -4747,19 +4750,22 @@
         <v>212</v>
       </c>
       <c r="F64" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G64" t="s">
         <v>212</v>
       </c>
       <c r="H64" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I64" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J64" t="s">
         <v>21</v>
+      </c>
+      <c r="M64" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1">
@@ -4777,13 +4783,13 @@
         <v>50</v>
       </c>
       <c r="F65" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G65" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H65" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I65" t="s">
         <v>542</v>
@@ -4794,7 +4800,7 @@
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1">
       <c r="A66" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B66" t="s">
         <v>475</v>
@@ -4807,16 +4813,16 @@
         <v>222</v>
       </c>
       <c r="F66" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G66" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H66" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I66" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J66" t="s">
         <v>561</v>
@@ -4824,7 +4830,7 @@
     </row>
     <row r="67" spans="1:13" ht="15" customHeight="1">
       <c r="A67" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B67" t="s">
         <v>269</v>
@@ -4840,10 +4846,10 @@
         <v>270</v>
       </c>
       <c r="F67" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G67" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H67" t="s">
         <v>562</v>
@@ -4876,13 +4882,13 @@
         <v>232</v>
       </c>
       <c r="F68" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G68" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H68" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I68" t="s">
         <v>233</v>
@@ -4907,13 +4913,13 @@
         <v>212</v>
       </c>
       <c r="F69" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G69" t="s">
         <v>212</v>
       </c>
       <c r="H69" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I69" t="s">
         <v>544</v>
@@ -4923,7 +4929,9 @@
       </c>
       <c r="K69"/>
       <c r="L69"/>
-      <c r="M69"/>
+      <c r="M69" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="70" spans="1:13" ht="15" customHeight="1">
       <c r="A70" t="s">
@@ -4940,10 +4948,10 @@
         <v>270</v>
       </c>
       <c r="F70" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G70" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H70" t="s">
         <v>562</v>
@@ -4970,10 +4978,10 @@
         <v>50</v>
       </c>
       <c r="F71" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G71" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H71" t="s">
         <v>562</v>
@@ -4997,10 +5005,10 @@
         <v>265</v>
       </c>
       <c r="F72" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G72" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H72" t="s">
         <v>562</v>
@@ -5033,16 +5041,16 @@
         <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G73" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H73" t="s">
         <v>556</v>
       </c>
       <c r="I73" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>564</v>
@@ -5068,13 +5076,13 @@
         <v>77</v>
       </c>
       <c r="G74" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H74" t="s">
         <v>556</v>
       </c>
       <c r="I74" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J74" t="s">
         <v>21</v>
@@ -5095,22 +5103,22 @@
         <v>207</v>
       </c>
       <c r="F75" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G75" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H75" t="s">
         <v>556</v>
       </c>
       <c r="I75" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J75" t="s">
         <v>521</v>
       </c>
       <c r="M75" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15" customHeight="1">
@@ -5131,10 +5139,10 @@
         <v>50</v>
       </c>
       <c r="F76" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G76" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H76" t="s">
         <v>527</v>
@@ -5161,10 +5169,10 @@
         <v>306</v>
       </c>
       <c r="F77" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G77" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H77" t="s">
         <v>527</v>
@@ -5191,10 +5199,10 @@
         <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G78" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H78" t="s">
         <v>527</v>
@@ -5221,10 +5229,10 @@
         <v>273</v>
       </c>
       <c r="F79" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G79" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H79" t="s">
         <v>527</v>
@@ -5254,10 +5262,10 @@
         <v>50</v>
       </c>
       <c r="F80" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G80" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H80" t="s">
         <v>527</v>
@@ -5284,16 +5292,16 @@
         <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G81" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H81" t="s">
         <v>527</v>
       </c>
       <c r="I81" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J81" t="s">
         <v>564</v>
@@ -5314,10 +5322,10 @@
         <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G82" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H82" t="s">
         <v>527</v>
@@ -5326,7 +5334,7 @@
         <v>582</v>
       </c>
       <c r="J82" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15" customHeight="1">
@@ -5344,10 +5352,10 @@
         <v>19</v>
       </c>
       <c r="F83" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G83" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H83" t="s">
         <v>527</v>
@@ -5375,10 +5383,10 @@
         <v>50</v>
       </c>
       <c r="F84" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G84" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H84" t="s">
         <v>527</v>
@@ -5408,10 +5416,10 @@
         <v>219</v>
       </c>
       <c r="F85" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G85" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H85" t="s">
         <v>547</v>
@@ -5438,10 +5446,10 @@
         <v>247</v>
       </c>
       <c r="F86" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G86" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H86" t="s">
         <v>547</v>
@@ -5450,7 +5458,7 @@
         <v>385</v>
       </c>
       <c r="J86" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="15" customHeight="1">
@@ -5471,10 +5479,10 @@
         <v>434</v>
       </c>
       <c r="F87" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G87" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H87" t="s">
         <v>547</v>
@@ -5483,12 +5491,12 @@
         <v>435</v>
       </c>
       <c r="J87" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="15" customHeight="1">
       <c r="A88" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B88" t="s">
         <v>344</v>
@@ -5501,10 +5509,10 @@
         <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G88" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H88" t="s">
         <v>576</v>
@@ -5531,7 +5539,7 @@
         <v>212</v>
       </c>
       <c r="F89" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G89" t="s">
         <v>212</v>
@@ -5540,10 +5548,10 @@
         <v>576</v>
       </c>
       <c r="I89" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J89" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="15" customHeight="1">
@@ -5561,10 +5569,10 @@
         <v>576</v>
       </c>
       <c r="I90" t="s">
+        <v>598</v>
+      </c>
+      <c r="J90" t="s">
         <v>599</v>
-      </c>
-      <c r="J90" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="91" spans="1:13" s="4" customFormat="1" ht="15" customHeight="1">
@@ -5583,16 +5591,16 @@
         <v>8</v>
       </c>
       <c r="F91" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G91" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H91" t="s">
         <v>576</v>
       </c>
       <c r="I91" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J91" t="s">
         <v>525</v>
@@ -5616,19 +5624,19 @@
         <v>50</v>
       </c>
       <c r="F92" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G92" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H92" t="s">
         <v>576</v>
       </c>
       <c r="I92" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J92" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="15" customHeight="1">
@@ -5646,16 +5654,16 @@
         <v>8</v>
       </c>
       <c r="F93" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G93" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H93" t="s">
         <v>576</v>
       </c>
       <c r="I93" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J93" t="s">
         <v>21</v>
@@ -5663,7 +5671,7 @@
     </row>
     <row r="94" spans="1:13" ht="15" customHeight="1">
       <c r="A94" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B94" t="s">
         <v>360</v>
@@ -5676,24 +5684,24 @@
         <v>361</v>
       </c>
       <c r="F94" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G94" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H94" t="s">
         <v>576</v>
       </c>
       <c r="I94" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J94" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="95" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A95" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B95" t="s">
         <v>22</v>
@@ -5709,10 +5717,10 @@
         <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G95" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H95" t="s">
         <v>576</v>
@@ -5727,7 +5735,7 @@
     </row>
     <row r="96" spans="1:13" ht="15" customHeight="1">
       <c r="A96" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B96" t="s">
         <v>22</v>
@@ -5743,7 +5751,7 @@
         <v>484</v>
       </c>
       <c r="G96" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H96" t="s">
         <v>576</v>
@@ -5754,7 +5762,7 @@
     </row>
     <row r="97" spans="1:13" ht="15" customHeight="1">
       <c r="A97" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B97" t="s">
         <v>22</v>
@@ -5770,10 +5778,10 @@
         <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G97" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H97" t="s">
         <v>576</v>
@@ -5800,10 +5808,10 @@
         <v>416</v>
       </c>
       <c r="F98" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G98" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H98" t="s">
         <v>590</v>
@@ -5815,7 +5823,7 @@
         <v>548</v>
       </c>
       <c r="M98" t="s">
-        <v>591</v>
+        <v>730</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15" customHeight="1">
@@ -5836,7 +5844,7 @@
         <v>413</v>
       </c>
       <c r="F99" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G99" t="s">
         <v>212</v>
@@ -5866,10 +5874,10 @@
         <v>59</v>
       </c>
       <c r="F100" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G100" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H100" t="s">
         <v>590</v>
@@ -5883,10 +5891,10 @@
     </row>
     <row r="101" spans="1:13" ht="15" customHeight="1">
       <c r="A101" t="s">
+        <v>606</v>
+      </c>
+      <c r="B101" t="s">
         <v>607</v>
-      </c>
-      <c r="B101" t="s">
-        <v>608</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="1"/>
@@ -5902,7 +5910,7 @@
         <v>525</v>
       </c>
       <c r="M101" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="15" customHeight="1">
@@ -5917,13 +5925,13 @@
         <v xml:space="preserve">Jerry Yang </v>
       </c>
       <c r="E102" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F102" t="s">
         <v>77</v>
       </c>
       <c r="G102" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H102" t="s">
         <v>590</v>
@@ -5953,10 +5961,10 @@
         <v>15</v>
       </c>
       <c r="G103" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H103" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I103" t="s">
         <v>523</v>
@@ -5983,10 +5991,10 @@
         <v>15</v>
       </c>
       <c r="G104" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H104" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I104" t="s">
         <v>523</v>
@@ -6007,7 +6015,7 @@
         <v xml:space="preserve">Craig Heatley </v>
       </c>
       <c r="E105" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F105" t="s">
         <v>366</v>
@@ -6016,10 +6024,10 @@
         <v>366</v>
       </c>
       <c r="H105" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J105" s="4" t="s">
         <v>21</v>
@@ -6040,19 +6048,19 @@
         <v>8</v>
       </c>
       <c r="F106" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G106" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H106" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I106" t="s">
         <v>228</v>
       </c>
       <c r="J106" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="15" customHeight="1">
@@ -6073,16 +6081,16 @@
         <v>205</v>
       </c>
       <c r="F107" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G107" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H107" t="s">
         <v>539</v>
       </c>
       <c r="I107" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="J107" t="s">
         <v>525</v>
@@ -6106,10 +6114,10 @@
         <v>71</v>
       </c>
       <c r="F108" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G108" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H108" t="s">
         <v>539</v>
@@ -6142,13 +6150,13 @@
         <v>416</v>
       </c>
       <c r="F109" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G109" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H109" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I109" t="s">
         <v>417</v>
@@ -6176,10 +6184,10 @@
         <v>495</v>
       </c>
       <c r="G110" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H110" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I110" t="s">
         <v>496</v>
@@ -6193,7 +6201,7 @@
     </row>
     <row r="111" spans="1:13" ht="15" customHeight="1">
       <c r="A111" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B111" t="s">
         <v>387</v>
@@ -6209,19 +6217,19 @@
         <v>129</v>
       </c>
       <c r="F111" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G111" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H111" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I111" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J111" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="112" spans="1:13">
@@ -6229,7 +6237,7 @@
         <v>269</v>
       </c>
       <c r="B112" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="1"/>
@@ -6242,21 +6250,24 @@
         <v>439</v>
       </c>
       <c r="G112" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H112" t="s">
         <v>522</v>
       </c>
       <c r="I112" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="J112" t="s">
         <v>525</v>
       </c>
+      <c r="M112" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B113" t="s">
         <v>255</v>
@@ -6272,16 +6283,16 @@
         <v>50</v>
       </c>
       <c r="F113" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G113" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H113" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I113" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="J113" t="s">
         <v>561</v>

</xml_diff>

<commit_message>
112 --> 111 ;)
also filter classing for different toplines depending on view
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Unconfirmed" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Confirmed!$A$1:$M$216</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Confirmed!$A$1:$M$215</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="728">
   <si>
     <t>Last</t>
   </si>
@@ -1238,9 +1238,6 @@
     <t>Menk</t>
   </si>
   <si>
-    <t>Roundtree</t>
-  </si>
-  <si>
     <t xml:space="preserve">Augusta </t>
   </si>
   <si>
@@ -1890,12 +1887,6 @@
   </si>
   <si>
     <t>Government</t>
-  </si>
-  <si>
-    <t>Sheriff</t>
-  </si>
-  <si>
-    <t>Richmond County</t>
   </si>
   <si>
     <t>Reagan Administration</t>
@@ -2285,8 +2276,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2343,7 +2338,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2368,6 +2363,8 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2392,6 +2389,8 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2726,10 +2725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M113"/>
+  <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2749,16 +2748,16 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D1" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -2767,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -2779,10 +2778,10 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="L1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="M1" t="s">
         <v>16</v>
@@ -2803,19 +2802,19 @@
         <v>238</v>
       </c>
       <c r="F2" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G2" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="H2" t="s">
+        <v>551</v>
+      </c>
+      <c r="I2" t="s">
         <v>552</v>
       </c>
-      <c r="I2" t="s">
-        <v>553</v>
-      </c>
       <c r="J2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
@@ -2826,7 +2825,7 @@
         <v>389</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">A3&amp;" "&amp;B3&amp;" "&amp;C3</f>
+        <f t="shared" ref="D3:D65" si="0">A3&amp;" "&amp;B3&amp;" "&amp;C3</f>
         <v xml:space="preserve">Bruce  Lilly </v>
       </c>
       <c r="E3" t="s">
@@ -2836,24 +2835,24 @@
         <v>391</v>
       </c>
       <c r="G3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="H3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I3" t="s">
         <v>392</v>
       </c>
       <c r="J3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2863,19 +2862,19 @@
         <v>273</v>
       </c>
       <c r="F4" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G4" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="H4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1">
@@ -2893,19 +2892,19 @@
         <v>247</v>
       </c>
       <c r="F5" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="G5" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="H5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I5" t="s">
         <v>248</v>
       </c>
       <c r="J5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
@@ -2913,7 +2912,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -2926,24 +2925,24 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G6" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" t="s">
         <v>426</v>
-      </c>
-      <c r="B7" t="s">
-        <v>427</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -2953,19 +2952,19 @@
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="G7" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="H7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
@@ -2983,13 +2982,13 @@
         <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G8" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I8" t="s">
         <v>398</v>
@@ -3010,25 +3009,25 @@
         <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="G9" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="H9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I9" t="s">
+        <v>558</v>
+      </c>
+      <c r="J9" t="s">
+        <v>547</v>
+      </c>
+      <c r="K9" t="s">
         <v>559</v>
       </c>
-      <c r="J9" t="s">
-        <v>548</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>560</v>
-      </c>
-      <c r="L9" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
@@ -3049,16 +3048,16 @@
         <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="H10" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="I10" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="J10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1">
@@ -3066,29 +3065,29 @@
         <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Robert O'Block </v>
       </c>
       <c r="E11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F11" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="G11" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="H11" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="I11" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="J11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1">
@@ -3106,16 +3105,16 @@
         <v>235</v>
       </c>
       <c r="F12" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G12" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J12" t="s">
         <v>21</v>
@@ -3123,7 +3122,7 @@
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
@@ -3142,16 +3141,16 @@
         <v>371</v>
       </c>
       <c r="G13" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="H13" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
@@ -3172,19 +3171,19 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G14" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J14" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
@@ -3205,19 +3204,19 @@
         <v>212</v>
       </c>
       <c r="F15" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="G15" t="s">
         <v>212</v>
       </c>
       <c r="H15" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="J15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3236,19 +3235,19 @@
         <v>115</v>
       </c>
       <c r="F16" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="G16" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="H16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I16" t="s">
+        <v>593</v>
+      </c>
+      <c r="J16" t="s">
         <v>594</v>
-      </c>
-      <c r="J16" t="s">
-        <v>595</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>
@@ -3275,16 +3274,16 @@
         <v>348</v>
       </c>
       <c r="G17" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K17"/>
       <c r="L17"/>
@@ -3308,19 +3307,19 @@
         <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G18" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="H18" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I18" t="s">
+        <v>531</v>
+      </c>
+      <c r="J18" t="s">
         <v>532</v>
-      </c>
-      <c r="J18" t="s">
-        <v>533</v>
       </c>
       <c r="K18"/>
       <c r="L18"/>
@@ -3328,7 +3327,7 @@
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="A19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3341,19 +3340,19 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="G19" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="H19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I19" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="J19" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
@@ -3374,16 +3373,16 @@
         <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="H20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1">
@@ -3401,19 +3400,19 @@
         <v>222</v>
       </c>
       <c r="F21" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="G21" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="H21" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I21" t="s">
+        <v>548</v>
+      </c>
+      <c r="J21" t="s">
         <v>549</v>
-      </c>
-      <c r="J21" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1">
@@ -3437,13 +3436,13 @@
         <v>354</v>
       </c>
       <c r="G22" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="H22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I22" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1">
@@ -3464,27 +3463,27 @@
         <v>273</v>
       </c>
       <c r="F23" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G23" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="H23" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I23" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="J23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1">
       <c r="A24" t="s">
+        <v>465</v>
+      </c>
+      <c r="B24" t="s">
         <v>466</v>
-      </c>
-      <c r="B24" t="s">
-        <v>467</v>
       </c>
       <c r="C24" t="s">
         <v>31</v>
@@ -3494,22 +3493,22 @@
         <v xml:space="preserve">Will Nicholson Jr. </v>
       </c>
       <c r="E24" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F24" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="G24" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="H24" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I24" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J24" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -3530,19 +3529,19 @@
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G25" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H25" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J25" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K25"/>
       <c r="L25"/>
@@ -3563,19 +3562,19 @@
         <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="G26" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="H26" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I26" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1">
@@ -3594,19 +3593,19 @@
         <v>261</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -3630,24 +3629,24 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="H28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I28" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="J28" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M28" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B29" t="s">
         <v>386</v>
@@ -3660,22 +3659,22 @@
         <v>Francis A. Townsend III</v>
       </c>
       <c r="E29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F29" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="G29" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="H29" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I29" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="J29" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1">
@@ -3696,16 +3695,16 @@
         <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="H30" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I30" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J30" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1">
@@ -3713,7 +3712,7 @@
         <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -3723,27 +3722,27 @@
         <v>244</v>
       </c>
       <c r="F31" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="G31" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="H31" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="I31" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" t="s">
+        <v>406</v>
+      </c>
+      <c r="B32" t="s">
         <v>407</v>
-      </c>
-      <c r="B32" t="s">
-        <v>408</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -3753,27 +3752,27 @@
         <v>273</v>
       </c>
       <c r="F32" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G32" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="H32" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="I32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B33" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -3783,27 +3782,27 @@
         <v>273</v>
       </c>
       <c r="F33" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G33" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="H33" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="I33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1">
       <c r="A34" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B34" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
@@ -3813,27 +3812,27 @@
         <v xml:space="preserve">Harris V. Morrisette Jr. </v>
       </c>
       <c r="E34" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F34" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="G34" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="H34" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="I34" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="J34" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
       <c r="A35" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B35" t="s">
         <v>380</v>
@@ -3846,16 +3845,16 @@
         <v>129</v>
       </c>
       <c r="F35" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="G35" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="H35" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="I35" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J35" t="s">
         <v>21</v>
@@ -3866,7 +3865,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" t="str">
@@ -3874,22 +3873,22 @@
         <v xml:space="preserve">George Wislar </v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>662</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>693</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>643</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>487</v>
-      </c>
       <c r="J36" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -3916,21 +3915,21 @@
         <v>27</v>
       </c>
       <c r="H37" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I37" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="J37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15" customHeight="1">
       <c r="A38" t="s">
+        <v>498</v>
+      </c>
+      <c r="B38" t="s">
         <v>499</v>
-      </c>
-      <c r="B38" t="s">
-        <v>500</v>
       </c>
       <c r="C38" t="s">
         <v>31</v>
@@ -3940,22 +3939,22 @@
         <v xml:space="preserve">Jack  Burke Jr. </v>
       </c>
       <c r="E38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F38" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G38" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="H38" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I38" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J38" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1">
@@ -3976,19 +3975,19 @@
         <v>50</v>
       </c>
       <c r="F39" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G39" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H39" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I39" t="s">
         <v>65</v>
       </c>
       <c r="J39" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1">
@@ -4009,13 +4008,13 @@
         <v>69</v>
       </c>
       <c r="G40" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="H40" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J40" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1">
@@ -4023,7 +4022,7 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -4033,22 +4032,22 @@
         <v>William Farish III</v>
       </c>
       <c r="E41" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F41" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G41" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="H41" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I41" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="J41" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
@@ -4067,19 +4066,19 @@
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G42" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H42" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I42" t="s">
         <v>382</v>
       </c>
       <c r="J42" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
@@ -4103,233 +4102,229 @@
         <v>77</v>
       </c>
       <c r="G43" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="H43" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I43" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="J43" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="M43" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15" customHeight="1">
       <c r="A44" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="B44" t="s">
-        <v>404</v>
-      </c>
-      <c r="C44"/>
+        <v>476</v>
+      </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Richard Roundtree </v>
+        <v xml:space="preserve">George  Shultz </v>
       </c>
       <c r="E44" t="s">
-        <v>405</v>
+        <v>477</v>
       </c>
       <c r="F44" t="s">
-        <v>662</v>
+        <v>77</v>
       </c>
       <c r="G44" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="H44" t="s">
+        <v>620</v>
+      </c>
+      <c r="I44" t="s">
         <v>621</v>
       </c>
-      <c r="I44" t="s">
-        <v>623</v>
-      </c>
       <c r="J44" t="s">
-        <v>622</v>
-      </c>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44"/>
+        <v>478</v>
+      </c>
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1">
       <c r="A45" t="s">
-        <v>349</v>
+        <v>267</v>
       </c>
       <c r="B45" t="s">
-        <v>477</v>
+        <v>268</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">George  Shultz </v>
+        <v xml:space="preserve">J. Bransford Wallace </v>
       </c>
       <c r="E45" t="s">
-        <v>478</v>
+        <v>232</v>
       </c>
       <c r="F45" t="s">
-        <v>77</v>
+        <v>668</v>
       </c>
       <c r="G45" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="H45" t="s">
-        <v>621</v>
+        <v>527</v>
       </c>
       <c r="I45" t="s">
-        <v>624</v>
+        <v>564</v>
       </c>
       <c r="J45" t="s">
-        <v>479</v>
+        <v>534</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="B46" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">J. Bransford Wallace </v>
+        <v xml:space="preserve">Edward Herlihy </v>
       </c>
       <c r="E46" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="F46" t="s">
-        <v>671</v>
+        <v>643</v>
       </c>
       <c r="G46" t="s">
-        <v>708</v>
+        <v>212</v>
       </c>
       <c r="H46" t="s">
-        <v>528</v>
-      </c>
-      <c r="I46" t="s">
-        <v>565</v>
+        <v>568</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="J46" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1">
       <c r="A47" t="s">
-        <v>239</v>
+        <v>435</v>
       </c>
       <c r="B47" t="s">
-        <v>299</v>
+        <v>436</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Edward Herlihy </v>
+        <v xml:space="preserve">Harold  Andersen </v>
       </c>
       <c r="E47" t="s">
-        <v>212</v>
+        <v>437</v>
       </c>
       <c r="F47" t="s">
-        <v>646</v>
+        <v>438</v>
       </c>
       <c r="G47" t="s">
-        <v>212</v>
+        <v>715</v>
       </c>
       <c r="H47" t="s">
-        <v>569</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>300</v>
+        <v>556</v>
+      </c>
+      <c r="I47" t="s">
+        <v>684</v>
       </c>
       <c r="J47" t="s">
-        <v>521</v>
+        <v>547</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1">
       <c r="A48" t="s">
-        <v>436</v>
+        <v>394</v>
       </c>
       <c r="B48" t="s">
-        <v>437</v>
+        <v>306</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Harold  Andersen </v>
+        <v xml:space="preserve">Nick  Evans </v>
       </c>
       <c r="E48" t="s">
-        <v>438</v>
+        <v>50</v>
       </c>
       <c r="F48" t="s">
-        <v>439</v>
+        <v>659</v>
       </c>
       <c r="G48" t="s">
-        <v>718</v>
+        <v>690</v>
       </c>
       <c r="H48" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I48" t="s">
-        <v>687</v>
+        <v>395</v>
       </c>
       <c r="J48" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="15" customHeight="1">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
-        <v>394</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>306</v>
+        <v>256</v>
+      </c>
+      <c r="C49" t="s">
+        <v>31</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Nick  Evans </v>
+        <v xml:space="preserve">James Hoak Jr. </v>
       </c>
       <c r="E49" t="s">
-        <v>50</v>
+        <v>257</v>
       </c>
       <c r="F49" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="G49" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H49" t="s">
+        <v>556</v>
+      </c>
+      <c r="I49" t="s">
         <v>557</v>
       </c>
-      <c r="I49" t="s">
-        <v>395</v>
-      </c>
       <c r="J49" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15" customHeight="1">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s">
-        <v>256</v>
-      </c>
-      <c r="C50" t="s">
-        <v>31</v>
+        <v>373</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">James Hoak Jr. </v>
+        <v xml:space="preserve">David Ingram </v>
       </c>
       <c r="E50" t="s">
-        <v>257</v>
+        <v>374</v>
       </c>
       <c r="F50" t="s">
-        <v>658</v>
+        <v>668</v>
       </c>
       <c r="G50" t="s">
-        <v>697</v>
+        <v>705</v>
       </c>
       <c r="H50" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I50" t="s">
-        <v>558</v>
+        <v>375</v>
       </c>
       <c r="J50" t="s">
         <v>21</v>
@@ -4337,1622 +4332,1626 @@
     </row>
     <row r="51" spans="1:13" ht="15" customHeight="1">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>462</v>
       </c>
       <c r="B51" t="s">
-        <v>373</v>
+        <v>463</v>
+      </c>
+      <c r="C51" t="s">
+        <v>31</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">David Ingram </v>
+        <v xml:space="preserve">Clifford  Kirtland Jr. </v>
       </c>
       <c r="E51" t="s">
-        <v>374</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>671</v>
+        <v>659</v>
       </c>
       <c r="G51" t="s">
-        <v>708</v>
+        <v>690</v>
       </c>
       <c r="H51" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I51" t="s">
-        <v>375</v>
+        <v>464</v>
       </c>
       <c r="J51" t="s">
-        <v>21</v>
+        <v>547</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15" customHeight="1">
       <c r="A52" t="s">
-        <v>463</v>
+        <v>516</v>
       </c>
       <c r="B52" t="s">
-        <v>464</v>
-      </c>
-      <c r="C52" t="s">
-        <v>31</v>
+        <v>517</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Clifford  Kirtland Jr. </v>
-      </c>
-      <c r="E52" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" t="s">
-        <v>662</v>
-      </c>
-      <c r="G52" t="s">
-        <v>693</v>
+        <v xml:space="preserve">Rob Light </v>
       </c>
       <c r="H52" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I52" t="s">
-        <v>465</v>
+        <v>518</v>
       </c>
       <c r="J52" t="s">
-        <v>548</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15" customHeight="1">
       <c r="A53" t="s">
-        <v>517</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>518</v>
+        <v>313</v>
+      </c>
+      <c r="C53" t="s">
+        <v>314</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Rob Light </v>
+        <v>William Morris IV</v>
+      </c>
+      <c r="E53" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" t="s">
+        <v>659</v>
+      </c>
+      <c r="G53" t="s">
+        <v>690</v>
       </c>
       <c r="H53" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I53" t="s">
-        <v>519</v>
+        <v>315</v>
       </c>
       <c r="J53" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15" customHeight="1">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>217</v>
       </c>
       <c r="B54" t="s">
         <v>313</v>
       </c>
       <c r="C54" t="s">
-        <v>314</v>
+        <v>23</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>William Morris IV</v>
+        <v>William  Morris III</v>
       </c>
       <c r="E54" t="s">
         <v>50</v>
       </c>
       <c r="F54" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G54" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H54" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I54" t="s">
         <v>315</v>
       </c>
       <c r="J54" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15" customHeight="1">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>608</v>
       </c>
       <c r="B55" t="s">
         <v>313</v>
       </c>
-      <c r="C55" t="s">
-        <v>23</v>
-      </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>William  Morris III</v>
+        <v xml:space="preserve">Charles H. Morris </v>
       </c>
       <c r="E55" t="s">
-        <v>50</v>
+        <v>405</v>
       </c>
       <c r="F55" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G55" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I55" t="s">
-        <v>315</v>
+        <v>644</v>
       </c>
       <c r="J55" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="15" customHeight="1">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A56" t="s">
-        <v>609</v>
+        <v>622</v>
       </c>
       <c r="B56" t="s">
-        <v>313</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="C56"/>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Charles H. Morris </v>
+        <v xml:space="preserve">Turner Simkins </v>
       </c>
       <c r="E56" t="s">
-        <v>406</v>
+        <v>50</v>
       </c>
       <c r="F56" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G56" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H56" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I56" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="J56" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+        <v>563</v>
+      </c>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+    </row>
+    <row r="57" spans="1:13" ht="15" customHeight="1">
       <c r="A57" t="s">
-        <v>625</v>
+        <v>251</v>
       </c>
       <c r="B57" t="s">
-        <v>323</v>
-      </c>
-      <c r="C57"/>
+        <v>386</v>
+      </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Turner Simkins </v>
+        <v xml:space="preserve">Ronald Townsend </v>
       </c>
       <c r="E57" t="s">
-        <v>50</v>
+        <v>343</v>
       </c>
       <c r="F57" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="G57" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H57" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I57" t="s">
-        <v>654</v>
+        <v>630</v>
       </c>
       <c r="J57" t="s">
-        <v>564</v>
-      </c>
-      <c r="K57"/>
-      <c r="L57"/>
-      <c r="M57"/>
+        <v>574</v>
+      </c>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1">
       <c r="A58" t="s">
-        <v>251</v>
+        <v>454</v>
       </c>
       <c r="B58" t="s">
-        <v>386</v>
+        <v>455</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Ronald Townsend </v>
+        <v xml:space="preserve">H. Ray  Finney </v>
       </c>
       <c r="E58" t="s">
-        <v>343</v>
+        <v>50</v>
       </c>
       <c r="F58" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="G58" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="H58" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
       <c r="I58" t="s">
-        <v>633</v>
+        <v>587</v>
       </c>
       <c r="J58" t="s">
-        <v>575</v>
+        <v>588</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1">
       <c r="A59" t="s">
-        <v>455</v>
+        <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>456</v>
+        <v>305</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">H. Ray  Finney </v>
+        <v xml:space="preserve">Paul Herzwurm </v>
       </c>
       <c r="E59" t="s">
-        <v>50</v>
+        <v>306</v>
       </c>
       <c r="F59" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G59" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H59" t="s">
+        <v>569</v>
+      </c>
+      <c r="I59" t="s">
+        <v>304</v>
+      </c>
+      <c r="J59" t="s">
         <v>570</v>
-      </c>
-      <c r="I59" t="s">
-        <v>588</v>
-      </c>
-      <c r="J59" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>302</v>
       </c>
       <c r="B60" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Paul Herzwurm </v>
+        <v xml:space="preserve">W. Howard  Hudson </v>
       </c>
       <c r="E60" t="s">
-        <v>306</v>
+        <v>50</v>
       </c>
       <c r="F60" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G60" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H60" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I60" t="s">
         <v>304</v>
       </c>
       <c r="J60" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15" customHeight="1">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">W. Howard  Hudson </v>
+        <v xml:space="preserve">Robert Waller </v>
       </c>
       <c r="E61" t="s">
-        <v>50</v>
+        <v>308</v>
       </c>
       <c r="F61" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="G61" t="s">
-        <v>693</v>
+        <v>705</v>
       </c>
       <c r="H61" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I61" t="s">
-        <v>304</v>
+        <v>724</v>
       </c>
       <c r="J61" t="s">
+        <v>574</v>
+      </c>
+      <c r="K61" t="s">
+        <v>309</v>
+      </c>
+      <c r="L61" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>307</v>
+        <v>449</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Robert Waller </v>
+        <v xml:space="preserve">John  Dobbs </v>
       </c>
       <c r="E62" t="s">
         <v>308</v>
       </c>
       <c r="F62" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="G62" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="H62" t="s">
-        <v>570</v>
+        <v>642</v>
       </c>
       <c r="I62" t="s">
-        <v>727</v>
-      </c>
-      <c r="J62" t="s">
-        <v>575</v>
-      </c>
-      <c r="K62" t="s">
-        <v>309</v>
-      </c>
-      <c r="L62" t="s">
-        <v>572</v>
+        <v>585</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="15" customHeight="1">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>625</v>
       </c>
       <c r="B63" t="s">
-        <v>450</v>
+        <v>626</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">John  Dobbs </v>
+        <v xml:space="preserve">Stanley Druckenmiller </v>
       </c>
       <c r="E63" t="s">
-        <v>308</v>
+        <v>212</v>
       </c>
       <c r="F63" t="s">
-        <v>671</v>
+        <v>643</v>
       </c>
       <c r="G63" t="s">
-        <v>708</v>
+        <v>212</v>
       </c>
       <c r="H63" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="I63" t="s">
-        <v>586</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>530</v>
+        <v>627</v>
+      </c>
+      <c r="J63" t="s">
+        <v>21</v>
+      </c>
+      <c r="M63" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1">
       <c r="A64" t="s">
-        <v>628</v>
+        <v>208</v>
       </c>
       <c r="B64" t="s">
-        <v>629</v>
+        <v>209</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Stanley Druckenmiller </v>
+        <v xml:space="preserve">Jefferson  Knox </v>
       </c>
       <c r="E64" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
       <c r="F64" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="G64" t="s">
-        <v>212</v>
+        <v>690</v>
       </c>
       <c r="H64" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="I64" t="s">
-        <v>630</v>
+        <v>541</v>
       </c>
       <c r="J64" t="s">
-        <v>21</v>
-      </c>
-      <c r="M64" t="s">
-        <v>730</v>
+        <v>542</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>617</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>474</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Jefferson  Knox </v>
+        <v xml:space="preserve">Ogden Mills Phipps </v>
       </c>
       <c r="E65" t="s">
-        <v>50</v>
+        <v>222</v>
       </c>
       <c r="F65" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="G65" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H65" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="I65" t="s">
-        <v>542</v>
+        <v>646</v>
       </c>
       <c r="J65" t="s">
-        <v>543</v>
+        <v>560</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1">
       <c r="A66" t="s">
-        <v>618</v>
+        <v>723</v>
       </c>
       <c r="B66" t="s">
-        <v>475</v>
+        <v>269</v>
+      </c>
+      <c r="C66" t="s">
+        <v>54</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Ogden Mills Phipps </v>
+        <f t="shared" ref="D66:D112" si="1">A66&amp;" "&amp;B66&amp;" "&amp;C66</f>
+        <v>William K. Warren Jr.</v>
       </c>
       <c r="E66" t="s">
-        <v>222</v>
+        <v>270</v>
       </c>
       <c r="F66" t="s">
-        <v>658</v>
+        <v>669</v>
       </c>
       <c r="G66" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="H66" t="s">
-        <v>645</v>
+        <v>561</v>
       </c>
       <c r="I66" t="s">
-        <v>649</v>
+        <v>565</v>
       </c>
       <c r="J66" t="s">
-        <v>561</v>
+        <v>566</v>
+      </c>
+      <c r="K66" t="s">
+        <v>565</v>
+      </c>
+      <c r="L66" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="15" customHeight="1">
       <c r="A67" t="s">
-        <v>726</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
-        <v>269</v>
-      </c>
-      <c r="C67" t="s">
-        <v>54</v>
+        <v>231</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D113" si="1">A67&amp;" "&amp;B67&amp;" "&amp;C67</f>
-        <v>William K. Warren Jr.</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Toby Wilt </v>
       </c>
       <c r="E67" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="F67" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="G67" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="H67" t="s">
-        <v>562</v>
+        <v>642</v>
       </c>
       <c r="I67" t="s">
-        <v>566</v>
+        <v>233</v>
       </c>
       <c r="J67" t="s">
-        <v>567</v>
-      </c>
-      <c r="K67" t="s">
-        <v>566</v>
-      </c>
-      <c r="L67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="15" customHeight="1">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A68" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>231</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="C68"/>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Toby Wilt </v>
+        <v xml:space="preserve">Dirk Ziff </v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="F68" t="s">
-        <v>671</v>
+        <v>643</v>
       </c>
       <c r="G68" t="s">
-        <v>708</v>
+        <v>212</v>
       </c>
       <c r="H68" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="I68" t="s">
-        <v>233</v>
+        <v>543</v>
       </c>
       <c r="J68" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+        <v>544</v>
+      </c>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15" customHeight="1">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>301</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
-      </c>
-      <c r="C69"/>
+        <v>490</v>
+      </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Dirk Ziff </v>
+        <v xml:space="preserve">Robert  Berry </v>
       </c>
       <c r="E69" t="s">
-        <v>212</v>
+        <v>270</v>
       </c>
       <c r="F69" t="s">
-        <v>646</v>
+        <v>669</v>
       </c>
       <c r="G69" t="s">
-        <v>212</v>
+        <v>706</v>
       </c>
       <c r="H69" t="s">
-        <v>645</v>
+        <v>561</v>
       </c>
       <c r="I69" t="s">
-        <v>544</v>
+        <v>577</v>
       </c>
       <c r="J69" t="s">
-        <v>545</v>
-      </c>
-      <c r="K69"/>
-      <c r="L69"/>
-      <c r="M69" t="s">
-        <v>730</v>
+        <v>524</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="15" customHeight="1">
       <c r="A70" t="s">
-        <v>301</v>
+        <v>503</v>
       </c>
       <c r="B70" t="s">
-        <v>491</v>
+        <v>504</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Robert  Berry </v>
+        <v xml:space="preserve">Clayton  Boardman </v>
       </c>
       <c r="E70" t="s">
-        <v>270</v>
+        <v>50</v>
       </c>
       <c r="F70" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="G70" t="s">
-        <v>709</v>
+        <v>690</v>
       </c>
       <c r="H70" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I70" t="s">
         <v>578</v>
       </c>
-      <c r="J70" t="s">
-        <v>525</v>
-      </c>
     </row>
     <row r="71" spans="1:13" ht="15" customHeight="1">
       <c r="A71" t="s">
-        <v>504</v>
+        <v>263</v>
       </c>
       <c r="B71" t="s">
-        <v>505</v>
+        <v>264</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Clayton  Boardman </v>
+        <v xml:space="preserve">Jack Vickers </v>
       </c>
       <c r="E71" t="s">
-        <v>50</v>
+        <v>265</v>
       </c>
       <c r="F71" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="G71" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
       <c r="H71" t="s">
+        <v>561</v>
+      </c>
+      <c r="I71" t="s">
         <v>562</v>
       </c>
-      <c r="I71" t="s">
-        <v>579</v>
+      <c r="J71" t="s">
+        <v>560</v>
+      </c>
+      <c r="K71" t="s">
+        <v>266</v>
+      </c>
+      <c r="L71" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="15" customHeight="1">
       <c r="A72" t="s">
-        <v>263</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>264</v>
+        <v>215</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Jack Vickers </v>
+        <v xml:space="preserve">David Dorman </v>
       </c>
       <c r="E72" t="s">
-        <v>265</v>
+        <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
       <c r="G72" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="H72" t="s">
-        <v>562</v>
+        <v>652</v>
       </c>
       <c r="I72" t="s">
-        <v>563</v>
+        <v>228</v>
       </c>
       <c r="J72" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="K72" t="s">
-        <v>266</v>
-      </c>
-      <c r="L72" t="s">
-        <v>564</v>
+        <v>602</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="15" customHeight="1">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">David Dorman </v>
+        <v xml:space="preserve">Bradford Freeman </v>
       </c>
       <c r="E73" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="F73" t="s">
-        <v>662</v>
+        <v>77</v>
       </c>
       <c r="G73" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="H73" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I73" t="s">
-        <v>603</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
+        <v>677</v>
+      </c>
+      <c r="J73" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="74" spans="1:13" ht="15" customHeight="1">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>355</v>
       </c>
       <c r="B74" t="s">
-        <v>249</v>
+        <v>356</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Bradford Freeman </v>
+        <v xml:space="preserve">Darla  Moore </v>
       </c>
       <c r="E74" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="F74" t="s">
-        <v>77</v>
+        <v>667</v>
       </c>
       <c r="G74" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
       <c r="H74" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I74" t="s">
         <v>680</v>
       </c>
       <c r="J74" t="s">
-        <v>21</v>
+        <v>520</v>
+      </c>
+      <c r="M74" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="15" customHeight="1">
       <c r="A75" t="s">
-        <v>355</v>
+        <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>356</v>
+        <v>234</v>
+      </c>
+      <c r="C75" t="s">
+        <v>31</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Darla  Moore </v>
+        <v xml:space="preserve">Thomas Blanchard Jr. </v>
       </c>
       <c r="E75" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="F75" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
       <c r="G75" t="s">
-        <v>707</v>
+        <v>690</v>
       </c>
       <c r="H75" t="s">
-        <v>556</v>
+        <v>526</v>
       </c>
       <c r="I75" t="s">
-        <v>683</v>
+        <v>572</v>
       </c>
       <c r="J75" t="s">
-        <v>521</v>
-      </c>
-      <c r="M75" t="s">
-        <v>608</v>
+        <v>529</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15" customHeight="1">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>418</v>
       </c>
       <c r="B76" t="s">
-        <v>234</v>
-      </c>
-      <c r="C76" t="s">
-        <v>31</v>
+        <v>419</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Thomas Blanchard Jr. </v>
+        <v xml:space="preserve">Stephen  Brown </v>
       </c>
       <c r="E76" t="s">
-        <v>50</v>
+        <v>306</v>
       </c>
       <c r="F76" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G76" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H76" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I76" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="J76" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="15" customHeight="1">
       <c r="A77" t="s">
-        <v>419</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>420</v>
+        <v>491</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Stephen  Brown </v>
+        <v xml:space="preserve">Thomas Cousins </v>
       </c>
       <c r="E77" t="s">
-        <v>306</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G77" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H77" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I77" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="J77" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="15" customHeight="1">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>367</v>
       </c>
       <c r="B78" t="s">
-        <v>492</v>
+        <v>460</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Thomas Cousins </v>
+        <v xml:space="preserve">John Harris </v>
       </c>
       <c r="E78" t="s">
-        <v>8</v>
+        <v>273</v>
       </c>
       <c r="F78" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="G78" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="H78" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I78" t="s">
-        <v>582</v>
+        <v>461</v>
       </c>
       <c r="J78" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="15" customHeight="1">
       <c r="A79" t="s">
-        <v>367</v>
+        <v>48</v>
       </c>
       <c r="B79" t="s">
-        <v>461</v>
+        <v>49</v>
+      </c>
+      <c r="C79" t="s">
+        <v>31</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">John Harris </v>
+        <v xml:space="preserve">Eugene  Howerdd Jr. </v>
       </c>
       <c r="E79" t="s">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="F79" t="s">
         <v>659</v>
       </c>
       <c r="G79" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H79" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I79" t="s">
-        <v>462</v>
+        <v>51</v>
       </c>
       <c r="J79" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="15" customHeight="1">
       <c r="A80" t="s">
-        <v>48</v>
+        <v>301</v>
       </c>
       <c r="B80" t="s">
-        <v>49</v>
-      </c>
-      <c r="C80" t="s">
-        <v>31</v>
+        <v>376</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Eugene  Howerdd Jr. </v>
+        <v xml:space="preserve">Robert  Johnston </v>
       </c>
       <c r="E80" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="F80" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G80" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H80" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I80" t="s">
-        <v>51</v>
+        <v>678</v>
       </c>
       <c r="J80" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="15" customHeight="1">
       <c r="A81" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
       <c r="B81" t="s">
-        <v>376</v>
+        <v>288</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Robert  Johnston </v>
+        <v xml:space="preserve">John  McColl </v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G81" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H81" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I81" t="s">
-        <v>681</v>
+        <v>581</v>
       </c>
       <c r="J81" t="s">
-        <v>564</v>
+        <v>594</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="15" customHeight="1">
       <c r="A82" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>288</v>
+        <v>18</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">John  McColl </v>
+        <v xml:space="preserve">Fred Ridley </v>
       </c>
       <c r="E82" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="G82" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I82" t="s">
-        <v>582</v>
+        <v>525</v>
       </c>
       <c r="J82" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="15" customHeight="1">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>322</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="C83"/>
       <c r="D83" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Fred Ridley </v>
+        <v xml:space="preserve">Leroy Simkins </v>
       </c>
       <c r="E83" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F83" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="G83" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="H83" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I83" t="s">
-        <v>526</v>
+        <v>573</v>
       </c>
       <c r="J83" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+        <v>574</v>
+      </c>
+      <c r="K83"/>
+      <c r="L83"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:13" ht="15" customHeight="1">
       <c r="A84" t="s">
-        <v>322</v>
+        <v>217</v>
       </c>
       <c r="B84" t="s">
-        <v>323</v>
-      </c>
-      <c r="C84"/>
+        <v>218</v>
+      </c>
       <c r="D84" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Leroy Simkins </v>
+        <v xml:space="preserve">William  Howell </v>
       </c>
       <c r="E84" t="s">
-        <v>50</v>
+        <v>219</v>
       </c>
       <c r="F84" t="s">
-        <v>662</v>
+        <v>670</v>
       </c>
       <c r="G84" t="s">
-        <v>693</v>
+        <v>708</v>
       </c>
       <c r="H84" t="s">
-        <v>527</v>
+        <v>546</v>
       </c>
       <c r="I84" t="s">
-        <v>574</v>
+        <v>220</v>
       </c>
       <c r="J84" t="s">
-        <v>575</v>
-      </c>
-      <c r="K84"/>
-      <c r="L84"/>
-      <c r="M84"/>
+        <v>547</v>
+      </c>
     </row>
     <row r="85" spans="1:13" ht="15" customHeight="1">
       <c r="A85" t="s">
-        <v>217</v>
+        <v>383</v>
       </c>
       <c r="B85" t="s">
-        <v>218</v>
+        <v>384</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">William  Howell </v>
+        <v xml:space="preserve">Lawrence  Pugh </v>
       </c>
       <c r="E85" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="F85" t="s">
-        <v>673</v>
+        <v>655</v>
       </c>
       <c r="G85" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="H85" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I85" t="s">
-        <v>220</v>
+        <v>385</v>
       </c>
       <c r="J85" t="s">
-        <v>548</v>
+        <v>618</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="15" customHeight="1">
       <c r="A86" t="s">
-        <v>383</v>
+        <v>516</v>
       </c>
       <c r="B86" t="s">
-        <v>384</v>
+        <v>432</v>
+      </c>
+      <c r="C86" t="s">
+        <v>31</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Lawrence  Pugh </v>
+        <v xml:space="preserve">Rob Spilman Jr. </v>
       </c>
       <c r="E86" t="s">
-        <v>247</v>
+        <v>433</v>
       </c>
       <c r="F86" t="s">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="G86" t="s">
-        <v>697</v>
+        <v>605</v>
       </c>
       <c r="H86" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I86" t="s">
-        <v>385</v>
+        <v>434</v>
       </c>
       <c r="J86" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="15" customHeight="1">
       <c r="A87" t="s">
-        <v>517</v>
+        <v>722</v>
       </c>
       <c r="B87" t="s">
-        <v>433</v>
-      </c>
-      <c r="C87" t="s">
-        <v>31</v>
+        <v>344</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Rob Spilman Jr. </v>
+        <v xml:space="preserve">Pat Battle </v>
       </c>
       <c r="E87" t="s">
-        <v>434</v>
+        <v>8</v>
       </c>
       <c r="F87" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="G87" t="s">
-        <v>606</v>
+        <v>690</v>
       </c>
       <c r="H87" t="s">
-        <v>547</v>
+        <v>575</v>
       </c>
       <c r="I87" t="s">
-        <v>435</v>
+        <v>576</v>
       </c>
       <c r="J87" t="s">
-        <v>626</v>
+        <v>560</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="15" customHeight="1">
       <c r="A88" t="s">
-        <v>725</v>
+        <v>505</v>
       </c>
       <c r="B88" t="s">
-        <v>344</v>
+        <v>506</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Pat Battle </v>
+        <v xml:space="preserve">Roger Goodell </v>
       </c>
       <c r="E88" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="F88" t="s">
-        <v>662</v>
+        <v>643</v>
       </c>
       <c r="G88" t="s">
-        <v>693</v>
+        <v>212</v>
       </c>
       <c r="H88" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I88" t="s">
-        <v>577</v>
+        <v>591</v>
       </c>
       <c r="J88" t="s">
-        <v>561</v>
+        <v>590</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="15" customHeight="1">
       <c r="A89" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="B89" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Roger Goodell </v>
-      </c>
-      <c r="E89" t="s">
-        <v>212</v>
-      </c>
-      <c r="F89" t="s">
-        <v>646</v>
-      </c>
-      <c r="G89" t="s">
-        <v>212</v>
+        <v xml:space="preserve">Lou  Holtz </v>
       </c>
       <c r="H89" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I89" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="J89" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="15" customHeight="1">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A90" t="s">
-        <v>512</v>
+        <v>423</v>
       </c>
       <c r="B90" t="s">
-        <v>513</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="C90"/>
       <c r="D90" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Lou  Holtz </v>
+        <v xml:space="preserve">Terence McGuirk </v>
+      </c>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
+        <v>659</v>
+      </c>
+      <c r="G90" t="s">
+        <v>690</v>
       </c>
       <c r="H90" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I90" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="J90" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" s="4" customFormat="1" ht="15" customHeight="1">
+        <v>524</v>
+      </c>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+    </row>
+    <row r="91" spans="1:13" ht="15" customHeight="1">
       <c r="A91" t="s">
-        <v>424</v>
+        <v>258</v>
       </c>
       <c r="B91" t="s">
-        <v>425</v>
-      </c>
-      <c r="C91"/>
+        <v>259</v>
+      </c>
       <c r="D91" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Terence McGuirk </v>
+        <v xml:space="preserve">J. Fleming Norvell </v>
       </c>
       <c r="E91" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F91" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G91" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H91" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I91" t="s">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="J91" t="s">
-        <v>525</v>
-      </c>
-      <c r="K91"/>
-      <c r="L91"/>
-      <c r="M91"/>
+        <v>598</v>
+      </c>
     </row>
     <row r="92" spans="1:13" ht="15" customHeight="1">
       <c r="A92" t="s">
-        <v>258</v>
+        <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>259</v>
+        <v>6</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">J. Fleming Norvell </v>
+        <v xml:space="preserve">William Payne </v>
       </c>
       <c r="E92" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="F92" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="G92" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="H92" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I92" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="J92" t="s">
-        <v>599</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="15" customHeight="1">
       <c r="A93" t="s">
-        <v>7</v>
+        <v>628</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>360</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">William Payne </v>
+        <v xml:space="preserve">Lynn C. Swann </v>
       </c>
       <c r="E93" t="s">
-        <v>8</v>
+        <v>361</v>
       </c>
       <c r="F93" t="s">
         <v>662</v>
       </c>
       <c r="G93" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="H93" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I93" t="s">
-        <v>617</v>
+        <v>591</v>
       </c>
       <c r="J93" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="15" customHeight="1">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A94" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="B94" t="s">
-        <v>360</v>
+        <v>22</v>
+      </c>
+      <c r="C94" t="s">
+        <v>23</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Lynn C. Swann </v>
+        <v>Danny Yates III</v>
       </c>
       <c r="E94" t="s">
-        <v>361</v>
+        <v>8</v>
       </c>
       <c r="F94" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="G94" t="s">
-        <v>700</v>
+        <v>690</v>
       </c>
       <c r="H94" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I94" t="s">
-        <v>592</v>
-      </c>
-      <c r="J94" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+        <v>528</v>
+      </c>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:13" ht="15" customHeight="1">
       <c r="A95" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B95" t="s">
         <v>22</v>
       </c>
-      <c r="C95" t="s">
-        <v>23</v>
-      </c>
       <c r="D95" t="str">
         <f t="shared" si="1"/>
-        <v>Danny Yates III</v>
+        <v xml:space="preserve">Dan Yates </v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>662</v>
+        <v>483</v>
       </c>
       <c r="G95" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H95" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I95" t="s">
-        <v>529</v>
-      </c>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95"/>
-      <c r="M95"/>
+        <v>528</v>
+      </c>
     </row>
     <row r="96" spans="1:13" ht="15" customHeight="1">
       <c r="A96" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="B96" t="s">
         <v>22</v>
       </c>
+      <c r="C96" t="s">
+        <v>31</v>
+      </c>
       <c r="D96" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Dan Yates </v>
+        <v xml:space="preserve">Charlie Yates Jr. </v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
       </c>
       <c r="F96" t="s">
-        <v>484</v>
+        <v>659</v>
       </c>
       <c r="G96" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="H96" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I96" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="15" customHeight="1">
       <c r="A97" t="s">
-        <v>637</v>
+        <v>513</v>
       </c>
       <c r="B97" t="s">
-        <v>22</v>
+        <v>514</v>
       </c>
       <c r="C97" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Charlie Yates Jr. </v>
+        <v>Bill  Gates III</v>
       </c>
       <c r="E97" t="s">
-        <v>8</v>
+        <v>415</v>
       </c>
       <c r="F97" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="G97" t="s">
-        <v>693</v>
+        <v>709</v>
       </c>
       <c r="H97" t="s">
-        <v>576</v>
+        <v>589</v>
       </c>
       <c r="I97" t="s">
-        <v>529</v>
+        <v>515</v>
+      </c>
+      <c r="J97" t="s">
+        <v>547</v>
+      </c>
+      <c r="M97" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="15" customHeight="1">
       <c r="A98" t="s">
-        <v>514</v>
+        <v>410</v>
       </c>
       <c r="B98" t="s">
-        <v>515</v>
+        <v>411</v>
       </c>
       <c r="C98" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="1"/>
-        <v>Bill  Gates III</v>
+        <v xml:space="preserve">Louis  Gerstner Jr. </v>
       </c>
       <c r="E98" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F98" t="s">
-        <v>675</v>
+        <v>643</v>
       </c>
       <c r="G98" t="s">
-        <v>712</v>
+        <v>212</v>
       </c>
       <c r="H98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I98" t="s">
-        <v>516</v>
+        <v>413</v>
       </c>
       <c r="J98" t="s">
-        <v>548</v>
-      </c>
-      <c r="M98" t="s">
-        <v>730</v>
+        <v>547</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15" customHeight="1">
       <c r="A99" t="s">
-        <v>411</v>
+        <v>293</v>
       </c>
       <c r="B99" t="s">
-        <v>412</v>
-      </c>
-      <c r="C99" t="s">
-        <v>31</v>
+        <v>294</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Louis  Gerstner Jr. </v>
+        <v xml:space="preserve">Samuel Palmisano </v>
       </c>
       <c r="E99" t="s">
+        <v>59</v>
+      </c>
+      <c r="F99" t="s">
+        <v>664</v>
+      </c>
+      <c r="G99" t="s">
+        <v>699</v>
+      </c>
+      <c r="H99" t="s">
+        <v>589</v>
+      </c>
+      <c r="I99" t="s">
         <v>413</v>
       </c>
-      <c r="F99" t="s">
-        <v>646</v>
-      </c>
-      <c r="G99" t="s">
-        <v>212</v>
-      </c>
-      <c r="H99" t="s">
-        <v>590</v>
-      </c>
-      <c r="I99" t="s">
-        <v>414</v>
-      </c>
       <c r="J99" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="15" customHeight="1">
       <c r="A100" t="s">
-        <v>293</v>
+        <v>605</v>
       </c>
       <c r="B100" t="s">
-        <v>294</v>
+        <v>606</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Samuel Palmisano </v>
-      </c>
-      <c r="E100" t="s">
-        <v>59</v>
-      </c>
-      <c r="F100" t="s">
-        <v>667</v>
-      </c>
-      <c r="G100" t="s">
-        <v>702</v>
+        <v xml:space="preserve">Virginia Rometty </v>
       </c>
       <c r="H100" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I100" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J100" t="s">
-        <v>548</v>
+        <v>524</v>
+      </c>
+      <c r="M100" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="15" customHeight="1">
       <c r="A101" t="s">
-        <v>606</v>
+        <v>509</v>
       </c>
       <c r="B101" t="s">
-        <v>607</v>
+        <v>75</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Virginia Rometty </v>
+        <v xml:space="preserve">Jerry Yang </v>
+      </c>
+      <c r="E101" t="s">
+        <v>632</v>
+      </c>
+      <c r="F101" t="s">
+        <v>77</v>
+      </c>
+      <c r="G101" t="s">
+        <v>695</v>
       </c>
       <c r="H101" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I101" t="s">
-        <v>414</v>
+        <v>510</v>
       </c>
       <c r="J101" t="s">
-        <v>525</v>
-      </c>
-      <c r="M101" t="s">
-        <v>608</v>
+        <v>547</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="15" customHeight="1">
       <c r="A102" t="s">
-        <v>510</v>
+        <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Jerry Yang </v>
+        <v xml:space="preserve">Joe Ford </v>
       </c>
       <c r="E102" t="s">
-        <v>635</v>
+        <v>14</v>
       </c>
       <c r="F102" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G102" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="H102" t="s">
-        <v>590</v>
+        <v>652</v>
       </c>
       <c r="I102" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="J102" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="15" customHeight="1">
       <c r="A103" t="s">
-        <v>12</v>
+        <v>372</v>
       </c>
       <c r="B103" t="s">
         <v>13</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Joe Ford </v>
+        <v xml:space="preserve">Scott Ford </v>
       </c>
       <c r="E103" t="s">
         <v>14</v>
@@ -5961,345 +5960,315 @@
         <v>15</v>
       </c>
       <c r="G103" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="H103" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="I103" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J103" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="15" customHeight="1">
       <c r="A104" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B104" t="s">
-        <v>13</v>
+        <v>365</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Scott Ford </v>
+        <v xml:space="preserve">Craig Heatley </v>
       </c>
       <c r="E104" t="s">
-        <v>14</v>
+        <v>716</v>
       </c>
       <c r="F104" t="s">
-        <v>15</v>
+        <v>366</v>
       </c>
       <c r="G104" t="s">
-        <v>706</v>
+        <v>366</v>
       </c>
       <c r="H104" t="s">
-        <v>655</v>
-      </c>
-      <c r="I104" t="s">
-        <v>523</v>
-      </c>
-      <c r="J104" t="s">
-        <v>548</v>
+        <v>652</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="15" customHeight="1">
       <c r="A105" t="s">
-        <v>364</v>
+        <v>226</v>
       </c>
       <c r="B105" t="s">
-        <v>365</v>
+        <v>227</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Craig Heatley </v>
+        <v xml:space="preserve">Ray  Robinson </v>
       </c>
       <c r="E105" t="s">
-        <v>719</v>
+        <v>8</v>
       </c>
       <c r="F105" t="s">
-        <v>366</v>
+        <v>659</v>
       </c>
       <c r="G105" t="s">
-        <v>366</v>
+        <v>690</v>
       </c>
       <c r="H105" t="s">
-        <v>655</v>
-      </c>
-      <c r="I105" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="J105" s="4" t="s">
-        <v>21</v>
+        <v>652</v>
+      </c>
+      <c r="I105" t="s">
+        <v>228</v>
+      </c>
+      <c r="J105" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="15" customHeight="1">
       <c r="A106" t="s">
-        <v>226</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>227</v>
+        <v>204</v>
+      </c>
+      <c r="C106" t="s">
+        <v>23</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Ray  Robinson </v>
+        <v>Robert Chapman III</v>
       </c>
       <c r="E106" t="s">
-        <v>8</v>
+        <v>205</v>
       </c>
       <c r="F106" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="G106" t="s">
-        <v>693</v>
+        <v>700</v>
       </c>
       <c r="H106" t="s">
-        <v>655</v>
+        <v>538</v>
       </c>
       <c r="I106" t="s">
-        <v>228</v>
+        <v>683</v>
       </c>
       <c r="J106" t="s">
-        <v>656</v>
+        <v>524</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="15" customHeight="1">
       <c r="A107" t="s">
-        <v>153</v>
+        <v>537</v>
       </c>
       <c r="B107" t="s">
-        <v>204</v>
+        <v>70</v>
       </c>
       <c r="C107" t="s">
         <v>23</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="1"/>
-        <v>Robert Chapman III</v>
+        <v>James C.  Self III</v>
       </c>
       <c r="E107" t="s">
-        <v>205</v>
+        <v>71</v>
       </c>
       <c r="F107" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="G107" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="H107" t="s">
+        <v>538</v>
+      </c>
+      <c r="I107" t="s">
         <v>539</v>
       </c>
-      <c r="I107" t="s">
-        <v>686</v>
-      </c>
       <c r="J107" t="s">
-        <v>525</v>
+        <v>529</v>
+      </c>
+      <c r="K107" t="s">
+        <v>72</v>
+      </c>
+      <c r="L107" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="15" customHeight="1">
       <c r="A108" t="s">
-        <v>538</v>
+        <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>70</v>
-      </c>
-      <c r="C108" t="s">
-        <v>23</v>
+        <v>414</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="1"/>
-        <v>James C.  Self III</v>
+        <v xml:space="preserve">Mark Pigott </v>
       </c>
       <c r="E108" t="s">
-        <v>71</v>
+        <v>415</v>
       </c>
       <c r="F108" t="s">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="G108" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="H108" t="s">
-        <v>539</v>
+        <v>648</v>
       </c>
       <c r="I108" t="s">
-        <v>540</v>
+        <v>416</v>
       </c>
       <c r="J108" t="s">
-        <v>530</v>
-      </c>
-      <c r="K108" t="s">
-        <v>72</v>
-      </c>
-      <c r="L108" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" ht="15" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A109" t="s">
-        <v>196</v>
+        <v>325</v>
       </c>
       <c r="B109" t="s">
-        <v>415</v>
-      </c>
+        <v>493</v>
+      </c>
+      <c r="C109"/>
       <c r="D109" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Mark Pigott </v>
+        <v xml:space="preserve">Charles Knight </v>
       </c>
       <c r="E109" t="s">
-        <v>416</v>
+        <v>32</v>
       </c>
       <c r="F109" t="s">
-        <v>675</v>
+        <v>494</v>
       </c>
       <c r="G109" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="H109" t="s">
-        <v>651</v>
+        <v>599</v>
       </c>
       <c r="I109" t="s">
-        <v>417</v>
+        <v>495</v>
       </c>
       <c r="J109" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1">
+        <v>547</v>
+      </c>
+      <c r="K109"/>
+      <c r="L109"/>
+      <c r="M109"/>
+    </row>
+    <row r="110" spans="1:13" ht="15" customHeight="1">
       <c r="A110" t="s">
-        <v>325</v>
+        <v>629</v>
       </c>
       <c r="B110" t="s">
-        <v>494</v>
-      </c>
-      <c r="C110"/>
+        <v>387</v>
+      </c>
+      <c r="C110" t="s">
+        <v>23</v>
+      </c>
       <c r="D110" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Charles Knight </v>
+        <v>Lee J. Styslinger III</v>
       </c>
       <c r="E110" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="F110" t="s">
-        <v>495</v>
+        <v>660</v>
       </c>
       <c r="G110" t="s">
-        <v>713</v>
+        <v>693</v>
       </c>
       <c r="H110" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I110" t="s">
-        <v>496</v>
+        <v>624</v>
       </c>
       <c r="J110" t="s">
-        <v>548</v>
-      </c>
-      <c r="K110"/>
-      <c r="L110"/>
-      <c r="M110"/>
-    </row>
-    <row r="111" spans="1:13" ht="15" customHeight="1">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
       <c r="A111" t="s">
-        <v>632</v>
+        <v>269</v>
       </c>
       <c r="B111" t="s">
-        <v>387</v>
-      </c>
-      <c r="C111" t="s">
-        <v>23</v>
+        <v>717</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="1"/>
-        <v>Lee J. Styslinger III</v>
+        <v xml:space="preserve">Warren Buffett </v>
       </c>
       <c r="E111" t="s">
-        <v>129</v>
+        <v>437</v>
       </c>
       <c r="F111" t="s">
-        <v>663</v>
+        <v>438</v>
       </c>
       <c r="G111" t="s">
-        <v>696</v>
+        <v>715</v>
       </c>
       <c r="H111" t="s">
-        <v>600</v>
+        <v>521</v>
       </c>
       <c r="I111" t="s">
-        <v>627</v>
+        <v>718</v>
       </c>
       <c r="J111" t="s">
-        <v>619</v>
+        <v>524</v>
+      </c>
+      <c r="M111" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" t="s">
-        <v>269</v>
+        <v>720</v>
       </c>
       <c r="B112" t="s">
-        <v>720</v>
+        <v>255</v>
+      </c>
+      <c r="C112" t="s">
+        <v>54</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Warren Buffett </v>
+        <v>Phil S.  Harison Jr.</v>
       </c>
       <c r="E112" t="s">
-        <v>438</v>
+        <v>50</v>
       </c>
       <c r="F112" t="s">
-        <v>439</v>
+        <v>659</v>
       </c>
       <c r="G112" t="s">
-        <v>718</v>
+        <v>690</v>
       </c>
       <c r="H112" t="s">
-        <v>522</v>
+        <v>726</v>
       </c>
       <c r="I112" t="s">
         <v>721</v>
       </c>
       <c r="J112" t="s">
-        <v>525</v>
-      </c>
-      <c r="M112" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" t="s">
-        <v>723</v>
-      </c>
-      <c r="B113" t="s">
-        <v>255</v>
-      </c>
-      <c r="C113" t="s">
-        <v>54</v>
-      </c>
-      <c r="D113" t="str">
-        <f t="shared" si="1"/>
-        <v>Phil S.  Harison Jr.</v>
-      </c>
-      <c r="E113" t="s">
-        <v>50</v>
-      </c>
-      <c r="F113" t="s">
-        <v>662</v>
-      </c>
-      <c r="G113" t="s">
-        <v>693</v>
-      </c>
-      <c r="H113" t="s">
-        <v>729</v>
-      </c>
-      <c r="I113" t="s">
-        <v>724</v>
-      </c>
-      <c r="J113" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M216">
+  <autoFilter ref="A1:M215">
     <sortState ref="A2:M216">
       <sortCondition ref="H1:H216"/>
     </sortState>
@@ -6347,14 +6316,14 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>444</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>445</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>371</v>
@@ -6371,17 +6340,17 @@
         <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -6389,14 +6358,14 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>447</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>448</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>213</v>
@@ -6410,10 +6379,10 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>488</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>489</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>31</v>
@@ -6422,7 +6391,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -6498,10 +6467,10 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>469</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>470</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
@@ -6519,21 +6488,21 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>471</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>472</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -6542,7 +6511,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>285</v>
@@ -6565,10 +6534,10 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>482</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>483</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>31</v>
@@ -6577,7 +6546,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -7794,10 +7763,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
+        <v>408</v>
+      </c>
+      <c r="B85" t="s">
         <v>409</v>
-      </c>
-      <c r="B85" t="s">
-        <v>410</v>
       </c>
       <c r="C85" t="s">
         <v>31</v>
@@ -7814,7 +7783,7 @@
         <v>217</v>
       </c>
       <c r="B86" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D86" t="s">
         <v>50</v>
@@ -7828,10 +7797,10 @@
         <v>326</v>
       </c>
       <c r="B87" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D87" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E87" t="s">
         <v>9</v>
@@ -7839,10 +7808,10 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
+        <v>421</v>
+      </c>
+      <c r="B88" t="s">
         <v>422</v>
-      </c>
-      <c r="B88" t="s">
-        <v>423</v>
       </c>
       <c r="C88" t="s">
         <v>31</v>
@@ -7856,13 +7825,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
+        <v>429</v>
+      </c>
+      <c r="B89" t="s">
         <v>430</v>
       </c>
-      <c r="B89" t="s">
+      <c r="D89" t="s">
         <v>431</v>
-      </c>
-      <c r="D89" t="s">
-        <v>432</v>
       </c>
       <c r="E89" t="s">
         <v>213</v>
@@ -7870,24 +7839,24 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
+        <v>439</v>
+      </c>
+      <c r="B90" t="s">
         <v>440</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>441</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>442</v>
-      </c>
-      <c r="E90" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
+        <v>458</v>
+      </c>
+      <c r="B91" t="s">
         <v>459</v>
-      </c>
-      <c r="B91" t="s">
-        <v>460</v>
       </c>
       <c r="C91" t="s">
         <v>23</v>
@@ -7904,10 +7873,10 @@
         <v>153</v>
       </c>
       <c r="B92" t="s">
+        <v>479</v>
+      </c>
+      <c r="D92" t="s">
         <v>480</v>
-      </c>
-      <c r="D92" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -7915,13 +7884,13 @@
         <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D93" t="s">
         <v>50</v>
       </c>
       <c r="E93" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -7929,27 +7898,27 @@
         <v>153</v>
       </c>
       <c r="B94" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D94" t="s">
         <v>8</v>
       </c>
       <c r="E94" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
+        <v>501</v>
+      </c>
+      <c r="B95" t="s">
         <v>502</v>
-      </c>
-      <c r="B95" t="s">
-        <v>503</v>
       </c>
       <c r="D95" t="s">
         <v>50</v>
       </c>
       <c r="E95" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring mapping views to display fields
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="728">
   <si>
     <t>Last</t>
   </si>
@@ -2727,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4011,6 +4011,9 @@
         <v>707</v>
       </c>
       <c r="H40" t="s">
+        <v>528</v>
+      </c>
+      <c r="I40" t="s">
         <v>528</v>
       </c>
       <c r="J40" t="s">

</xml_diff>

<commit_message>
Closes #6 v1.1 (111 to 118 names)
Correction and new names. Also restored nicknames that got lost from
spreadsheet.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="5160" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="744">
   <si>
     <t>Last</t>
   </si>
@@ -2208,6 +2208,54 @@
   </si>
   <si>
     <t>Billionaire</t>
+  </si>
+  <si>
+    <t>Hance</t>
+  </si>
+  <si>
+    <t>Carlyle Group</t>
+  </si>
+  <si>
+    <t>Operating Executive</t>
+  </si>
+  <si>
+    <t>O. Wayne</t>
+  </si>
+  <si>
+    <t>Isom</t>
+  </si>
+  <si>
+    <t>Weill Cornell Medical Center</t>
+  </si>
+  <si>
+    <t>Goode</t>
+  </si>
+  <si>
+    <t>Norfolk Southern Corp.</t>
+  </si>
+  <si>
+    <t>McKnight Construction Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savardi </t>
+  </si>
+  <si>
+    <t>Professional Services</t>
+  </si>
+  <si>
+    <t>Insperity</t>
+  </si>
+  <si>
+    <t>John "Jacko"</t>
+  </si>
+  <si>
+    <t>Maree</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Standard Bank Group</t>
   </si>
 </sst>
 </file>
@@ -2220,7 +2268,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2725,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3652,11 +3699,11 @@
         <v>386</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>Francis A. Townsend III</v>
+        <v>Francis A. Townsend Jr.</v>
       </c>
       <c r="E29" t="s">
         <v>480</v>
@@ -6268,6 +6315,170 @@
       </c>
       <c r="J112" t="s">
         <v>560</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" t="s">
+        <v>63</v>
+      </c>
+      <c r="B113" t="s">
+        <v>368</v>
+      </c>
+      <c r="E113" t="s">
+        <v>369</v>
+      </c>
+      <c r="F113" t="s">
+        <v>370</v>
+      </c>
+      <c r="G113" t="s">
+        <v>370</v>
+      </c>
+      <c r="H113" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" t="s">
+        <v>52</v>
+      </c>
+      <c r="B114" t="s">
+        <v>728</v>
+      </c>
+      <c r="C114" t="s">
+        <v>54</v>
+      </c>
+      <c r="F114" t="s">
+        <v>656</v>
+      </c>
+      <c r="G114" t="s">
+        <v>688</v>
+      </c>
+      <c r="H114" t="s">
+        <v>555</v>
+      </c>
+      <c r="I114" t="s">
+        <v>729</v>
+      </c>
+      <c r="J114" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" t="s">
+        <v>731</v>
+      </c>
+      <c r="B115" t="s">
+        <v>732</v>
+      </c>
+      <c r="E115" t="s">
+        <v>212</v>
+      </c>
+      <c r="F115" t="s">
+        <v>643</v>
+      </c>
+      <c r="G115" t="s">
+        <v>212</v>
+      </c>
+      <c r="H115" t="s">
+        <v>569</v>
+      </c>
+      <c r="I115" t="s">
+        <v>733</v>
+      </c>
+      <c r="J115" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" t="s">
+        <v>734</v>
+      </c>
+      <c r="H116" t="s">
+        <v>648</v>
+      </c>
+      <c r="I116" t="s">
+        <v>735</v>
+      </c>
+      <c r="J116" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" t="s">
+        <v>217</v>
+      </c>
+      <c r="B117" t="s">
+        <v>324</v>
+      </c>
+      <c r="E117" t="s">
+        <v>50</v>
+      </c>
+      <c r="F117" t="s">
+        <v>659</v>
+      </c>
+      <c r="G117" t="s">
+        <v>690</v>
+      </c>
+      <c r="H117" t="s">
+        <v>554</v>
+      </c>
+      <c r="I117" t="s">
+        <v>736</v>
+      </c>
+      <c r="J117" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" t="s">
+        <v>159</v>
+      </c>
+      <c r="B118" t="s">
+        <v>737</v>
+      </c>
+      <c r="F118" t="s">
+        <v>667</v>
+      </c>
+      <c r="G118" t="s">
+        <v>704</v>
+      </c>
+      <c r="H118" t="s">
+        <v>738</v>
+      </c>
+      <c r="I118" t="s">
+        <v>739</v>
+      </c>
+      <c r="J118" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" t="s">
+        <v>740</v>
+      </c>
+      <c r="B119" t="s">
+        <v>741</v>
+      </c>
+      <c r="E119" t="s">
+        <v>742</v>
+      </c>
+      <c r="F119" t="s">
+        <v>164</v>
+      </c>
+      <c r="G119" t="s">
+        <v>164</v>
+      </c>
+      <c r="H119" t="s">
+        <v>521</v>
+      </c>
+      <c r="I119" t="s">
+        <v>743</v>
+      </c>
+      <c r="J119" t="s">
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>